<commit_message>
added well header content model
added well header content model
</commit_message>
<xml_diff>
--- a/Links/Attribute-DataObject/Attribute-DataObject.xlsx
+++ b/Links/Attribute-DataObject/Attribute-DataObject.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="210">
   <si>
     <t>xs:dateTime</t>
   </si>
@@ -577,6 +577,87 @@
   </si>
   <si>
     <t>class/attribute/otherdistribution</t>
+  </si>
+  <si>
+    <t>class/data-object/well-header-occurrence</t>
+  </si>
+  <si>
+    <t>class/attribute/headeruri</t>
+  </si>
+  <si>
+    <t>class/attribute/othername</t>
+  </si>
+  <si>
+    <t>class/attribute/boreholename</t>
+  </si>
+  <si>
+    <t>class/attribute/mineralowner</t>
+  </si>
+  <si>
+    <t>class/attribute/driller</t>
+  </si>
+  <si>
+    <t>class/attribute/leasename</t>
+  </si>
+  <si>
+    <t>class/attribute/endeddrillingdate</t>
+  </si>
+  <si>
+    <t>class/attribute/drillingmethod</t>
+  </si>
+  <si>
+    <t>class/attribute/releasedate</t>
+  </si>
+  <si>
+    <t>class/attribute/drillertotaldepth</t>
+  </si>
+  <si>
+    <t>class/attribute/lengthunits</t>
+  </si>
+  <si>
+    <t>class/attribute/trueverticaldepth</t>
+  </si>
+  <si>
+    <t>class/attribute/elevationkb</t>
+  </si>
+  <si>
+    <t>class/attribute/elevationdf</t>
+  </si>
+  <si>
+    <t>class/attribute/elevationgl</t>
+  </si>
+  <si>
+    <t>class/attribute/bitdiametercollar</t>
+  </si>
+  <si>
+    <t>class/attribute/bitdiametertd</t>
+  </si>
+  <si>
+    <t>class/attribute/diameterunits</t>
+  </si>
+  <si>
+    <t>class/attribute/casinglogger</t>
+  </si>
+  <si>
+    <t>class/attribute/casingbottomdepthdriller</t>
+  </si>
+  <si>
+    <t>class/attribute/casingtopdepth</t>
+  </si>
+  <si>
+    <t>class/attribute/casingpipediameter</t>
+  </si>
+  <si>
+    <t>class/attribute/casingweight</t>
+  </si>
+  <si>
+    <t>class/attribute/casingweightunits</t>
+  </si>
+  <si>
+    <t>class/attribute/casingthickness</t>
+  </si>
+  <si>
+    <t>class/attribute/informationsource</t>
   </si>
 </sst>
 </file>
@@ -7137,10 +7218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H228"/>
+  <dimension ref="A1:H294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C209" sqref="C209"/>
+    <sheetView tabSelected="1" topLeftCell="A262" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B280" sqref="B280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12735,6 +12816,1656 @@
         <v>12</v>
       </c>
     </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A229" s="15" t="str">
+        <f>LOOKUP(B229,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B229" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C229" s="15" t="str">
+        <f>LOOKUP(D229,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>OBJECTID</v>
+      </c>
+      <c r="D229" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E229" s="6">
+        <v>1</v>
+      </c>
+      <c r="F229" s="5">
+        <v>1</v>
+      </c>
+      <c r="G229" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A230" s="15" t="str">
+        <f>LOOKUP(B230,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B230" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C230" s="15" t="str">
+        <f>LOOKUP(D230,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Header URI</v>
+      </c>
+      <c r="D230" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="E230" s="6">
+        <v>1</v>
+      </c>
+      <c r="F230" s="5">
+        <v>2</v>
+      </c>
+      <c r="G230" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A231" s="15" t="str">
+        <f>LOOKUP(B231,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B231" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C231" s="15" t="str">
+        <f>LOOKUP(D231,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Well Name</v>
+      </c>
+      <c r="D231" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E231" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F231" s="5">
+        <v>3</v>
+      </c>
+      <c r="G231" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A232" s="15" t="str">
+        <f>LOOKUP(B232,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B232" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C232" s="15" t="str">
+        <f>LOOKUP(D232,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>API No</v>
+      </c>
+      <c r="D232" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E232" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F232" s="5">
+        <v>4</v>
+      </c>
+      <c r="G232" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A233" s="15" t="str">
+        <f>LOOKUP(B233,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B233" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C233" s="15" t="str">
+        <f>LOOKUP(D233,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Label</v>
+      </c>
+      <c r="D233" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E233" s="6">
+        <v>1</v>
+      </c>
+      <c r="F233" s="5">
+        <v>5</v>
+      </c>
+      <c r="G233" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A234" s="15" t="str">
+        <f>LOOKUP(B234,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B234" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C234" s="15" t="str">
+        <f>LOOKUP(D234,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Other ID</v>
+      </c>
+      <c r="D234" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E234" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F234" s="5">
+        <v>6</v>
+      </c>
+      <c r="G234" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A235" s="15" t="str">
+        <f>LOOKUP(B235,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B235" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C235" s="15" t="str">
+        <f>LOOKUP(D235,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Other Name</v>
+      </c>
+      <c r="D235" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="E235" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F235" s="5">
+        <v>7</v>
+      </c>
+      <c r="G235" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A236" s="15" t="str">
+        <f>LOOKUP(B236,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B236" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C236" s="15" t="str">
+        <f>LOOKUP(D236,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Borehole Name</v>
+      </c>
+      <c r="D236" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="E236" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F236" s="5">
+        <v>8</v>
+      </c>
+      <c r="G236" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A237" s="15" t="str">
+        <f>LOOKUP(B237,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B237" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C237" s="15" t="str">
+        <f>LOOKUP(D237,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Parent Well URI</v>
+      </c>
+      <c r="D237" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E237" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F237" s="5">
+        <v>9</v>
+      </c>
+      <c r="G237" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A238" s="15" t="str">
+        <f>LOOKUP(B238,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B238" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C238" s="15" t="str">
+        <f>LOOKUP(D238,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Operator</v>
+      </c>
+      <c r="D238" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E238" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F238" s="5">
+        <v>10</v>
+      </c>
+      <c r="G238" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A239" s="15" t="str">
+        <f>LOOKUP(B239,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B239" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C239" s="15" t="str">
+        <f>LOOKUP(D239,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Mineral Owner</v>
+      </c>
+      <c r="D239" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="E239" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F239" s="5">
+        <v>11</v>
+      </c>
+      <c r="G239" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A240" s="15" t="str">
+        <f>LOOKUP(B240,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B240" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C240" s="15" t="str">
+        <f>LOOKUP(D240,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Driller</v>
+      </c>
+      <c r="D240" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E240" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F240" s="5">
+        <v>12</v>
+      </c>
+      <c r="G240" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A241" s="15" t="str">
+        <f>LOOKUP(B241,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B241" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C241" s="15" t="str">
+        <f>LOOKUP(D241,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Lease Name</v>
+      </c>
+      <c r="D241" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="E241" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F241" s="5">
+        <v>13</v>
+      </c>
+      <c r="G241" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A242" s="15" t="str">
+        <f>LOOKUP(B242,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B242" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C242" s="15" t="str">
+        <f>LOOKUP(D242,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Spud Date</v>
+      </c>
+      <c r="D242" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="E242" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F242" s="5">
+        <v>14</v>
+      </c>
+      <c r="G242" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A243" s="15" t="str">
+        <f>LOOKUP(B243,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B243" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C243" s="15" t="str">
+        <f>LOOKUP(D243,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Ended Drilling Date</v>
+      </c>
+      <c r="D243" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E243" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F243" s="5">
+        <v>15</v>
+      </c>
+      <c r="G243" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A244" s="15" t="str">
+        <f>LOOKUP(B244,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B244" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C244" s="15" t="str">
+        <f>LOOKUP(D244,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Drilling Method</v>
+      </c>
+      <c r="D244" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E244" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F244" s="5">
+        <v>16</v>
+      </c>
+      <c r="G244" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A245" s="15" t="str">
+        <f>LOOKUP(B245,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B245" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C245" s="15" t="str">
+        <f>LOOKUP(D245,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Well Type</v>
+      </c>
+      <c r="D245" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E245" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F245" s="5">
+        <v>17</v>
+      </c>
+      <c r="G245" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246" s="15" t="str">
+        <f>LOOKUP(B246,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B246" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C246" s="15" t="str">
+        <f>LOOKUP(D246,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Status</v>
+      </c>
+      <c r="D246" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E246" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F246" s="5">
+        <v>18</v>
+      </c>
+      <c r="G246" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A247" s="15" t="str">
+        <f>LOOKUP(B247,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B247" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C247" s="15" t="str">
+        <f>LOOKUP(D247,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Commodity Of Interest</v>
+      </c>
+      <c r="D247" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="E247" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F247" s="5">
+        <v>19</v>
+      </c>
+      <c r="G247" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248" s="15" t="str">
+        <f>LOOKUP(B248,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B248" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C248" s="15" t="str">
+        <f>LOOKUP(D248,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Status Date</v>
+      </c>
+      <c r="D248" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E248" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F248" s="5">
+        <v>20</v>
+      </c>
+      <c r="G248" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A249" s="15" t="str">
+        <f>LOOKUP(B249,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B249" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C249" s="15" t="str">
+        <f>LOOKUP(D249,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Function</v>
+      </c>
+      <c r="D249" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="E249" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F249" s="5">
+        <v>21</v>
+      </c>
+      <c r="G249" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A250" s="15" t="str">
+        <f>LOOKUP(B250,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B250" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C250" s="15" t="str">
+        <f>LOOKUP(D250,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Production status</v>
+      </c>
+      <c r="D250" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="E250" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F250" s="5">
+        <v>22</v>
+      </c>
+      <c r="G250" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A251" s="15" t="str">
+        <f>LOOKUP(B251,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B251" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C251" s="15" t="str">
+        <f>LOOKUP(D251,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v xml:space="preserve">Producing Interval </v>
+      </c>
+      <c r="D251" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="E251" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F251" s="5">
+        <v>23</v>
+      </c>
+      <c r="G251" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252" s="15" t="str">
+        <f>LOOKUP(B252,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B252" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C252" s="15" t="str">
+        <f>LOOKUP(D252,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Release Date</v>
+      </c>
+      <c r="D252" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="E252" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F252" s="5">
+        <v>24</v>
+      </c>
+      <c r="G252" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253" s="15" t="str">
+        <f>LOOKUP(B253,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B253" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C253" s="15" t="str">
+        <f>LOOKUP(D253,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>County</v>
+      </c>
+      <c r="D253" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E253" s="6">
+        <v>1</v>
+      </c>
+      <c r="F253" s="5">
+        <v>25</v>
+      </c>
+      <c r="G253" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254" s="15" t="str">
+        <f>LOOKUP(B254,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B254" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C254" s="15" t="str">
+        <f>LOOKUP(D254,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>State</v>
+      </c>
+      <c r="D254" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E254" s="6">
+        <v>1</v>
+      </c>
+      <c r="F254" s="5">
+        <v>26</v>
+      </c>
+      <c r="G254" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A255" s="15" t="str">
+        <f>LOOKUP(B255,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B255" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C255" s="15" t="str">
+        <f>LOOKUP(D255,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Field</v>
+      </c>
+      <c r="D255" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E255" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F255" s="5">
+        <v>27</v>
+      </c>
+      <c r="G255" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A256" s="15" t="str">
+        <f>LOOKUP(B256,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B256" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C256" s="15" t="str">
+        <f>LOOKUP(D256,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Other Location Name</v>
+      </c>
+      <c r="D256" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="E256" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F256" s="5">
+        <v>28</v>
+      </c>
+      <c r="G256" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A257" s="15" t="str">
+        <f>LOOKUP(B257,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B257" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C257" s="15" t="str">
+        <f>LOOKUP(D257,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>PLSS Meridians</v>
+      </c>
+      <c r="D257" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E257" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F257" s="5">
+        <v>29</v>
+      </c>
+      <c r="G257" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A258" s="15" t="str">
+        <f>LOOKUP(B258,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B258" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C258" s="15" t="str">
+        <f>LOOKUP(D258,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>TWP</v>
+      </c>
+      <c r="D258" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E258" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F258" s="5">
+        <v>30</v>
+      </c>
+      <c r="G258" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A259" s="15" t="str">
+        <f>LOOKUP(B259,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B259" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C259" s="15" t="str">
+        <f>LOOKUP(D259,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>RGE</v>
+      </c>
+      <c r="D259" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E259" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F259" s="5">
+        <v>31</v>
+      </c>
+      <c r="G259" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A260" s="15" t="str">
+        <f>LOOKUP(B260,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B260" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C260" s="15" t="str">
+        <f>LOOKUP(D260,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v xml:space="preserve">Section </v>
+      </c>
+      <c r="D260" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E260" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F260" s="5">
+        <v>32</v>
+      </c>
+      <c r="G260" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A261" s="15" t="str">
+        <f>LOOKUP(B261,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B261" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C261" s="15" t="str">
+        <f>LOOKUP(D261,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Section Part</v>
+      </c>
+      <c r="D261" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E261" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F261" s="5">
+        <v>33</v>
+      </c>
+      <c r="G261" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A262" s="15" t="str">
+        <f>LOOKUP(B262,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B262" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C262" s="15" t="str">
+        <f>LOOKUP(D262,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Parcel</v>
+      </c>
+      <c r="D262" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E262" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F262" s="5">
+        <v>34</v>
+      </c>
+      <c r="G262" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A263" s="15" t="str">
+        <f>LOOKUP(B263,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B263" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C263" s="15" t="str">
+        <f>LOOKUP(D263,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>UTM E</v>
+      </c>
+      <c r="D263" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E263" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F263" s="5">
+        <v>35</v>
+      </c>
+      <c r="G263" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A264" s="15" t="str">
+        <f>LOOKUP(B264,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B264" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C264" s="15" t="str">
+        <f>LOOKUP(D264,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>UTM N</v>
+      </c>
+      <c r="D264" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E264" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F264" s="5">
+        <v>36</v>
+      </c>
+      <c r="G264" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A265" s="15" t="str">
+        <f>LOOKUP(B265,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B265" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C265" s="15" t="str">
+        <f>LOOKUP(D265,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>UTM Datum Zone</v>
+      </c>
+      <c r="D265" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E265" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F265" s="5">
+        <v>37</v>
+      </c>
+      <c r="G265" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A266" s="15" t="str">
+        <f>LOOKUP(B266,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B266" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C266" s="15" t="str">
+        <f>LOOKUP(D266,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Latitude Degrees</v>
+      </c>
+      <c r="D266" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E266" s="6">
+        <v>1</v>
+      </c>
+      <c r="F266" s="5">
+        <v>38</v>
+      </c>
+      <c r="G266" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A267" s="15" t="str">
+        <f>LOOKUP(B267,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B267" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C267" s="15" t="str">
+        <f>LOOKUP(D267,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Longitude Degree</v>
+      </c>
+      <c r="D267" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E267" s="6">
+        <v>1</v>
+      </c>
+      <c r="F267" s="5">
+        <v>39</v>
+      </c>
+      <c r="G267" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A268" s="15" t="str">
+        <f>LOOKUP(B268,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B268" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C268" s="15" t="str">
+        <f>LOOKUP(D268,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>SRS</v>
+      </c>
+      <c r="D268" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E268" s="6">
+        <v>1</v>
+      </c>
+      <c r="F268" s="5">
+        <v>40</v>
+      </c>
+      <c r="G268" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A269" s="15" t="str">
+        <f>LOOKUP(B269,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B269" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C269" s="15" t="str">
+        <f>LOOKUP(D269,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Location Uncertainty Statement</v>
+      </c>
+      <c r="D269" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E269" s="6">
+        <v>1</v>
+      </c>
+      <c r="F269" s="5">
+        <v>41</v>
+      </c>
+      <c r="G269" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A270" s="15" t="str">
+        <f>LOOKUP(B270,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B270" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C270" s="15" t="str">
+        <f>LOOKUP(D270,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Location Uncertainty Code</v>
+      </c>
+      <c r="D270" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E270" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F270" s="5">
+        <v>42</v>
+      </c>
+      <c r="G270" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A271" s="15" t="str">
+        <f>LOOKUP(B271,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B271" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C271" s="15" t="str">
+        <f>LOOKUP(D271,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Location Uncertainty Radius</v>
+      </c>
+      <c r="D271" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E271" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F271" s="5">
+        <v>43</v>
+      </c>
+      <c r="G271" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A272" s="15" t="str">
+        <f>LOOKUP(B272,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B272" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C272" s="15" t="str">
+        <f>LOOKUP(D272,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Driller Total Depth</v>
+      </c>
+      <c r="D272" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="E272" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F272" s="5">
+        <v>44</v>
+      </c>
+      <c r="G272" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A273" s="15" t="str">
+        <f>LOOKUP(B273,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B273" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C273" s="15" t="str">
+        <f>LOOKUP(D273,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Depth Reference Point</v>
+      </c>
+      <c r="D273" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E273" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F273" s="5">
+        <v>45</v>
+      </c>
+      <c r="G273" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A274" s="15" t="str">
+        <f>LOOKUP(B274,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B274" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C274" s="15" t="str">
+        <f>LOOKUP(D274,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Length Units</v>
+      </c>
+      <c r="D274" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E274" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F274" s="5">
+        <v>46</v>
+      </c>
+      <c r="G274" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A275" s="15" t="str">
+        <f>LOOKUP(B275,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B275" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C275" s="15" t="str">
+        <f>LOOKUP(D275,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Well Bore Shape</v>
+      </c>
+      <c r="D275" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="E275" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F275" s="5">
+        <v>47</v>
+      </c>
+      <c r="G275" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A276" s="15" t="str">
+        <f>LOOKUP(B276,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B276" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C276" s="15" t="str">
+        <f>LOOKUP(D276,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>True Vertical Depth</v>
+      </c>
+      <c r="D276" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="E276" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F276" s="5">
+        <v>48</v>
+      </c>
+      <c r="G276" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A277" s="15" t="str">
+        <f>LOOKUP(B277,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B277" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C277" s="15" t="str">
+        <f>LOOKUP(D277,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Elevation KB</v>
+      </c>
+      <c r="D277" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="E277" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F277" s="5">
+        <v>49</v>
+      </c>
+      <c r="G277" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A278" s="15" t="str">
+        <f>LOOKUP(B278,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B278" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C278" s="15" t="str">
+        <f>LOOKUP(D278,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Elevation DF</v>
+      </c>
+      <c r="D278" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E278" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F278" s="5">
+        <v>50</v>
+      </c>
+      <c r="G278" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A279" s="15" t="str">
+        <f>LOOKUP(B279,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B279" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C279" s="15" t="str">
+        <f>LOOKUP(D279,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Elevation GL</v>
+      </c>
+      <c r="D279" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E279" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F279" s="5">
+        <v>51</v>
+      </c>
+      <c r="G279" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A280" s="15" t="str">
+        <f>LOOKUP(B280,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B280" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C280" s="15" t="str">
+        <f>LOOKUP(D280,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Formation TD</v>
+      </c>
+      <c r="D280" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E280" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F280" s="5">
+        <v>52</v>
+      </c>
+      <c r="G280" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A281" s="15" t="str">
+        <f>LOOKUP(B281,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B281" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C281" s="15" t="str">
+        <f>LOOKUP(D281,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Bit Diameter at Collar</v>
+      </c>
+      <c r="D281" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="E281" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F281" s="5">
+        <v>53</v>
+      </c>
+      <c r="G281" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A282" s="15" t="str">
+        <f>LOOKUP(B282,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B282" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C282" s="15" t="str">
+        <f>LOOKUP(D282,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Bit Diameter at TD</v>
+      </c>
+      <c r="D282" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E282" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F282" s="5">
+        <v>54</v>
+      </c>
+      <c r="G282" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A283" s="15" t="str">
+        <f>LOOKUP(B283,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B283" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C283" s="15" t="str">
+        <f>LOOKUP(D283,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Diameter Units</v>
+      </c>
+      <c r="D283" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="E283" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F283" s="5">
+        <v>55</v>
+      </c>
+      <c r="G283" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A284" s="15" t="str">
+        <f>LOOKUP(B284,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B284" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C284" s="15" t="str">
+        <f>LOOKUP(D284,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Related Resource</v>
+      </c>
+      <c r="D284" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E284" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F284" s="5">
+        <v>56</v>
+      </c>
+      <c r="G284" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A285" s="15" t="str">
+        <f>LOOKUP(B285,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B285" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C285" s="15" t="str">
+        <f>LOOKUP(D285,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Notes</v>
+      </c>
+      <c r="D285" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E285" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F285" s="5">
+        <v>57</v>
+      </c>
+      <c r="G285" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A286" s="15" t="str">
+        <f>LOOKUP(B286,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B286" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C286" s="15" t="str">
+        <f>LOOKUP(D286,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Casing Logger</v>
+      </c>
+      <c r="D286" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="E286" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F286" s="5">
+        <v>58</v>
+      </c>
+      <c r="G286" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A287" s="15" t="str">
+        <f>LOOKUP(B287,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B287" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C287" s="15" t="str">
+        <f>LOOKUP(D287,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Casing Bottom Depth Driller</v>
+      </c>
+      <c r="D287" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="E287" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F287" s="5">
+        <v>59</v>
+      </c>
+      <c r="G287" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A288" s="15" t="str">
+        <f>LOOKUP(B288,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B288" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C288" s="15" t="str">
+        <f>LOOKUP(D288,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Casing Top Depth</v>
+      </c>
+      <c r="D288" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="E288" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F288" s="5">
+        <v>60</v>
+      </c>
+      <c r="G288" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A289" s="15" t="str">
+        <f>LOOKUP(B289,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B289" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C289" s="15" t="str">
+        <f>LOOKUP(D289,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Casing Pipe Diameter</v>
+      </c>
+      <c r="D289" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E289" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F289" s="5">
+        <v>61</v>
+      </c>
+      <c r="G289" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A290" s="15" t="str">
+        <f>LOOKUP(B290,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B290" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C290" s="15" t="str">
+        <f>LOOKUP(D290,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Casing Weight</v>
+      </c>
+      <c r="D290" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="E290" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F290" s="5">
+        <v>62</v>
+      </c>
+      <c r="G290" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A291" s="15" t="str">
+        <f>LOOKUP(B291,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B291" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C291" s="15" t="str">
+        <f>LOOKUP(D291,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Casing Weight Units</v>
+      </c>
+      <c r="D291" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="E291" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F291" s="5">
+        <v>63</v>
+      </c>
+      <c r="G291" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A292" s="15" t="str">
+        <f>LOOKUP(B292,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B292" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C292" s="15" t="str">
+        <f>LOOKUP(D292,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Casing Thickness</v>
+      </c>
+      <c r="D292" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="E292" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F292" s="5">
+        <v>64</v>
+      </c>
+      <c r="G292" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A293" s="15" t="str">
+        <f>LOOKUP(B293,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B293" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C293" s="15" t="str">
+        <f>LOOKUP(D293,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Information Source</v>
+      </c>
+      <c r="D293" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="E293" s="6">
+        <v>1</v>
+      </c>
+      <c r="F293" s="5">
+        <v>65</v>
+      </c>
+      <c r="G293" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A294" s="15" t="str">
+        <f>LOOKUP(B294,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Header Occurrence</v>
+      </c>
+      <c r="B294" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C294" s="15" t="str">
+        <f>LOOKUP(D294,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Shape</v>
+      </c>
+      <c r="D294" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="E294" s="6">
+        <v>1</v>
+      </c>
+      <c r="F294" s="5">
+        <v>66</v>
+      </c>
+      <c r="G294" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added Well Fluid Production content model
added Well Fluid Production content model
</commit_message>
<xml_diff>
--- a/Links/Attribute-DataObject/Attribute-DataObject.xlsx
+++ b/Links/Attribute-DataObject/Attribute-DataObject.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="227">
   <si>
     <t>xs:dateTime</t>
   </si>
@@ -658,6 +658,57 @@
   </si>
   <si>
     <t>class/attribute/informationsource</t>
+  </si>
+  <si>
+    <t>class/attribute/recordname</t>
+  </si>
+  <si>
+    <t>class/attribute/producingfeature</t>
+  </si>
+  <si>
+    <t>class/attribute/intervalstartdatetime</t>
+  </si>
+  <si>
+    <t>class/attribute/intervalenddatetime</t>
+  </si>
+  <si>
+    <t>class/attribute/durationdays</t>
+  </si>
+  <si>
+    <t>class/attribute/permit</t>
+  </si>
+  <si>
+    <t>class/attribute/fluidtype</t>
+  </si>
+  <si>
+    <t>class/attribute/fluidvolume</t>
+  </si>
+  <si>
+    <t>class/attribute/fluidvolumeunits</t>
+  </si>
+  <si>
+    <t>class/attribute/temperature-f</t>
+  </si>
+  <si>
+    <t>class/attribute/pressure-psi</t>
+  </si>
+  <si>
+    <t>class/attribute/aggregationtype</t>
+  </si>
+  <si>
+    <t>class/attribute/measurementmethod</t>
+  </si>
+  <si>
+    <t>class/attribute/contactintervaltop</t>
+  </si>
+  <si>
+    <t>class/attribute/contactintervalbottom</t>
+  </si>
+  <si>
+    <t>class/attribute/relatedresources</t>
+  </si>
+  <si>
+    <t>class/data-object/well-fluid-production-result</t>
   </si>
 </sst>
 </file>
@@ -7218,10 +7269,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H294"/>
+  <dimension ref="A1:H329"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B280" sqref="B280"/>
+    <sheetView tabSelected="1" topLeftCell="A286" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G329" sqref="G329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14466,6 +14517,881 @@
         <v>12</v>
       </c>
     </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A295" s="15" t="str">
+        <f>LOOKUP(B295,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B295" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C295" s="15" t="str">
+        <f>LOOKUP(D295,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>OBJECTID</v>
+      </c>
+      <c r="D295" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E295" s="6">
+        <v>1</v>
+      </c>
+      <c r="F295" s="5">
+        <v>1</v>
+      </c>
+      <c r="G295" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A296" s="15" t="str">
+        <f>LOOKUP(B296,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B296" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C296" s="15" t="str">
+        <f>LOOKUP(D296,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Observation URI</v>
+      </c>
+      <c r="D296" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E296" s="6">
+        <v>1</v>
+      </c>
+      <c r="F296" s="5">
+        <v>2</v>
+      </c>
+      <c r="G296" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A297" s="15" t="str">
+        <f>LOOKUP(B297,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B297" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C297" s="15" t="str">
+        <f>LOOKUP(D297,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Record Name</v>
+      </c>
+      <c r="D297" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E297" s="6">
+        <v>1</v>
+      </c>
+      <c r="F297" s="5">
+        <v>3</v>
+      </c>
+      <c r="G297" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A298" s="15" t="str">
+        <f>LOOKUP(B298,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B298" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C298" s="15" t="str">
+        <f>LOOKUP(D298,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Notes</v>
+      </c>
+      <c r="D298" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E298" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F298" s="5">
+        <v>4</v>
+      </c>
+      <c r="G298" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A299" s="15" t="str">
+        <f>LOOKUP(B299,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B299" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C299" s="15" t="str">
+        <f>LOOKUP(D299,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Operator</v>
+      </c>
+      <c r="D299" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E299" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F299" s="5">
+        <v>5</v>
+      </c>
+      <c r="G299" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A300" s="15" t="str">
+        <f>LOOKUP(B300,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B300" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C300" s="15" t="str">
+        <f>LOOKUP(D300,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Producing Feature</v>
+      </c>
+      <c r="D300" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="E300" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F300" s="5">
+        <v>6</v>
+      </c>
+      <c r="G300" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A301" s="15" t="str">
+        <f>LOOKUP(B301,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B301" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C301" s="15" t="str">
+        <f>LOOKUP(D301,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Header URI</v>
+      </c>
+      <c r="D301" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="E301" s="6">
+        <v>1</v>
+      </c>
+      <c r="F301" s="5">
+        <v>7</v>
+      </c>
+      <c r="G301" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A302" s="15" t="str">
+        <f>LOOKUP(B302,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B302" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C302" s="15" t="str">
+        <f>LOOKUP(D302,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Well Name</v>
+      </c>
+      <c r="D302" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E302" s="6">
+        <v>1</v>
+      </c>
+      <c r="F302" s="5">
+        <v>8</v>
+      </c>
+      <c r="G302" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A303" s="15" t="str">
+        <f>LOOKUP(B303,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B303" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C303" s="15" t="str">
+        <f>LOOKUP(D303,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>API No</v>
+      </c>
+      <c r="D303" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E303" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F303" s="5">
+        <v>9</v>
+      </c>
+      <c r="G303" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A304" s="15" t="str">
+        <f>LOOKUP(B304,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B304" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C304" s="15" t="str">
+        <f>LOOKUP(D304,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Other ID</v>
+      </c>
+      <c r="D304" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E304" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F304" s="5">
+        <v>10</v>
+      </c>
+      <c r="G304" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A305" s="15" t="str">
+        <f>LOOKUP(B305,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B305" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C305" s="15" t="str">
+        <f>LOOKUP(D305,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>County</v>
+      </c>
+      <c r="D305" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E305" s="6">
+        <v>1</v>
+      </c>
+      <c r="F305" s="5">
+        <v>11</v>
+      </c>
+      <c r="G305" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A306" s="15" t="str">
+        <f>LOOKUP(B306,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B306" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C306" s="15" t="str">
+        <f>LOOKUP(D306,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>State</v>
+      </c>
+      <c r="D306" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E306" s="6">
+        <v>1</v>
+      </c>
+      <c r="F306" s="5">
+        <v>12</v>
+      </c>
+      <c r="G306" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A307" s="15" t="str">
+        <f>LOOKUP(B307,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B307" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C307" s="15" t="str">
+        <f>LOOKUP(D307,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Field</v>
+      </c>
+      <c r="D307" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E307" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F307" s="5">
+        <v>13</v>
+      </c>
+      <c r="G307" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A308" s="15" t="str">
+        <f>LOOKUP(B308,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B308" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C308" s="15" t="str">
+        <f>LOOKUP(D308,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Other Location Name</v>
+      </c>
+      <c r="D308" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="E308" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F308" s="5">
+        <v>14</v>
+      </c>
+      <c r="G308" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A309" s="15" t="str">
+        <f>LOOKUP(B309,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B309" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C309" s="15" t="str">
+        <f>LOOKUP(D309,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Latitude Degrees</v>
+      </c>
+      <c r="D309" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E309" s="6">
+        <v>1</v>
+      </c>
+      <c r="F309" s="5">
+        <v>15</v>
+      </c>
+      <c r="G309" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A310" s="15" t="str">
+        <f>LOOKUP(B310,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B310" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C310" s="15" t="str">
+        <f>LOOKUP(D310,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Longitude Degree</v>
+      </c>
+      <c r="D310" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E310" s="6">
+        <v>1</v>
+      </c>
+      <c r="F310" s="5">
+        <v>16</v>
+      </c>
+      <c r="G310" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A311" s="15" t="str">
+        <f>LOOKUP(B311,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B311" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C311" s="15" t="str">
+        <f>LOOKUP(D311,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>SRS</v>
+      </c>
+      <c r="D311" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E311" s="6">
+        <v>1</v>
+      </c>
+      <c r="F311" s="5">
+        <v>17</v>
+      </c>
+      <c r="G311" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A312" s="15" t="str">
+        <f>LOOKUP(B312,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B312" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C312" s="15" t="str">
+        <f>LOOKUP(D312,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Location Uncertainty Statement</v>
+      </c>
+      <c r="D312" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E312" s="6">
+        <v>1</v>
+      </c>
+      <c r="F312" s="5">
+        <v>18</v>
+      </c>
+      <c r="G312" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A313" s="15" t="str">
+        <f>LOOKUP(B313,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B313" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C313" s="15" t="str">
+        <f>LOOKUP(D313,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Interval Start Date Time</v>
+      </c>
+      <c r="D313" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="E313" s="6">
+        <v>1</v>
+      </c>
+      <c r="F313" s="5">
+        <v>19</v>
+      </c>
+      <c r="G313" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A314" s="15" t="str">
+        <f>LOOKUP(B314,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B314" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C314" s="15" t="str">
+        <f>LOOKUP(D314,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Interval End Date Time</v>
+      </c>
+      <c r="D314" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="E314" s="6">
+        <v>1</v>
+      </c>
+      <c r="F314" s="5">
+        <v>20</v>
+      </c>
+      <c r="G314" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A315" s="15" t="str">
+        <f>LOOKUP(B315,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B315" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C315" s="15" t="str">
+        <f>LOOKUP(D315,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Duration Days</v>
+      </c>
+      <c r="D315" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="E315" s="6">
+        <v>1</v>
+      </c>
+      <c r="F315" s="5">
+        <v>21</v>
+      </c>
+      <c r="G315" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A316" s="15" t="str">
+        <f>LOOKUP(B316,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B316" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C316" s="15" t="str">
+        <f>LOOKUP(D316,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Permit</v>
+      </c>
+      <c r="D316" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="E316" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F316" s="5">
+        <v>22</v>
+      </c>
+      <c r="G316" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A317" s="15" t="str">
+        <f>LOOKUP(B317,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B317" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C317" s="15" t="str">
+        <f>LOOKUP(D317,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Fluid Type</v>
+      </c>
+      <c r="D317" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="E317" s="6">
+        <v>1</v>
+      </c>
+      <c r="F317" s="5">
+        <v>23</v>
+      </c>
+      <c r="G317" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A318" s="15" t="str">
+        <f>LOOKUP(B318,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B318" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C318" s="15" t="str">
+        <f>LOOKUP(D318,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Fluid Volume</v>
+      </c>
+      <c r="D318" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="E318" s="6">
+        <v>1</v>
+      </c>
+      <c r="F318" s="5">
+        <v>24</v>
+      </c>
+      <c r="G318" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A319" s="15" t="str">
+        <f>LOOKUP(B319,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B319" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C319" s="15" t="str">
+        <f>LOOKUP(D319,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Fluid Volume Units</v>
+      </c>
+      <c r="D319" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="E319" s="6">
+        <v>1</v>
+      </c>
+      <c r="F319" s="5">
+        <v>25</v>
+      </c>
+      <c r="G319" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A320" s="15" t="str">
+        <f>LOOKUP(B320,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B320" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C320" s="15" t="str">
+        <f>LOOKUP(D320,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Temperature Fahrenheit</v>
+      </c>
+      <c r="D320" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="E320" s="6">
+        <v>1</v>
+      </c>
+      <c r="F320" s="5">
+        <v>26</v>
+      </c>
+      <c r="G320" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A321" s="15" t="str">
+        <f>LOOKUP(B321,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B321" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C321" s="15" t="str">
+        <f>LOOKUP(D321,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Pressure psi</v>
+      </c>
+      <c r="D321" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E321" s="6">
+        <v>1</v>
+      </c>
+      <c r="F321" s="5">
+        <v>27</v>
+      </c>
+      <c r="G321" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A322" s="15" t="str">
+        <f>LOOKUP(B322,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B322" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C322" s="15" t="str">
+        <f>LOOKUP(D322,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Aggregation Type</v>
+      </c>
+      <c r="D322" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="E322" s="6">
+        <v>1</v>
+      </c>
+      <c r="F322" s="5">
+        <v>28</v>
+      </c>
+      <c r="G322" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A323" s="15" t="str">
+        <f>LOOKUP(B323,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B323" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C323" s="15" t="str">
+        <f>LOOKUP(D323,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Measurement Method</v>
+      </c>
+      <c r="D323" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="E323" s="6">
+        <v>1</v>
+      </c>
+      <c r="F323" s="5">
+        <v>29</v>
+      </c>
+      <c r="G323" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A324" s="15" t="str">
+        <f>LOOKUP(B324,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B324" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C324" s="15" t="str">
+        <f>LOOKUP(D324,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Contact Interval Top</v>
+      </c>
+      <c r="D324" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="E324" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F324" s="5">
+        <v>30</v>
+      </c>
+      <c r="G324" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A325" s="15" t="str">
+        <f>LOOKUP(B325,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B325" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C325" s="15" t="str">
+        <f>LOOKUP(D325,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Contact Interval Bottom</v>
+      </c>
+      <c r="D325" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E325" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F325" s="5">
+        <v>31</v>
+      </c>
+      <c r="G325" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A326" s="15" t="str">
+        <f>LOOKUP(B326,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B326" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C326" s="15" t="str">
+        <f>LOOKUP(D326,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Source</v>
+      </c>
+      <c r="D326" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E326" s="6">
+        <v>1</v>
+      </c>
+      <c r="F326" s="5">
+        <v>32</v>
+      </c>
+      <c r="G326" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A327" s="15" t="str">
+        <f>LOOKUP(B327,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B327" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C327" s="15" t="str">
+        <f>LOOKUP(D327,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>MetadataURI</v>
+      </c>
+      <c r="D327" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E327" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F327" s="5">
+        <v>33</v>
+      </c>
+      <c r="G327" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="328" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A328" s="15" t="str">
+        <f>LOOKUP(B328,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B328" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C328" s="15" t="str">
+        <f>LOOKUP(D328,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Related Resources</v>
+      </c>
+      <c r="D328" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="E328" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F328" s="5">
+        <v>34</v>
+      </c>
+      <c r="G328" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A329" s="15" t="str">
+        <f>LOOKUP(B329,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Well Fluid Production Result</v>
+      </c>
+      <c r="B329" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C329" s="15" t="str">
+        <f>LOOKUP(D329,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Shape</v>
+      </c>
+      <c r="D329" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="E329" s="6">
+        <v>1</v>
+      </c>
+      <c r="F329" s="5">
+        <v>35</v>
+      </c>
+      <c r="G329" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added Volcanic Vents content model
added Volcanic Vents content model
</commit_message>
<xml_diff>
--- a/Links/Attribute-DataObject/Attribute-DataObject.xlsx
+++ b/Links/Attribute-DataObject/Attribute-DataObject.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="247">
   <si>
     <t>xs:dateTime</t>
   </si>
@@ -709,6 +709,66 @@
   </si>
   <si>
     <t>class/data-object/well-fluid-production-result</t>
+  </si>
+  <si>
+    <t>class/attribute/featureuri</t>
+  </si>
+  <si>
+    <t>class/attribute/volcventname</t>
+  </si>
+  <si>
+    <t>class/attribute/maplabel</t>
+  </si>
+  <si>
+    <t>class/attribute/description</t>
+  </si>
+  <si>
+    <t>class/attribute/featuretype</t>
+  </si>
+  <si>
+    <t>class/attribute/volcanicgroup</t>
+  </si>
+  <si>
+    <t>class/attribute/ventelevation</t>
+  </si>
+  <si>
+    <t>class/attribute/elevationuom</t>
+  </si>
+  <si>
+    <t>class/attribute/relatedfeature</t>
+  </si>
+  <si>
+    <t>class/attribute/geologichistory</t>
+  </si>
+  <si>
+    <t>class/attribute/youngestage</t>
+  </si>
+  <si>
+    <t>class/attribute/oldestage</t>
+  </si>
+  <si>
+    <t>class/attribute/youngestradiometricage-ma</t>
+  </si>
+  <si>
+    <t>class/attribute/oldestradiometricage-ma</t>
+  </si>
+  <si>
+    <t>class/attribute/ageuncertainty-ma</t>
+  </si>
+  <si>
+    <t>class/attribute/agesource</t>
+  </si>
+  <si>
+    <t>class/attribute/geologicunit</t>
+  </si>
+  <si>
+    <t>class/attribute/materialcomposition</t>
+  </si>
+  <si>
+    <t>class/attribute/flowtype</t>
+  </si>
+  <si>
+    <t>class/data-object/volcanic-vent-occurrence</t>
   </si>
 </sst>
 </file>
@@ -7269,10 +7329,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H329"/>
+  <dimension ref="A1:H363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G329" sqref="G329"/>
+    <sheetView tabSelected="1" topLeftCell="A337" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G326" sqref="G326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15392,6 +15452,856 @@
         <v>12</v>
       </c>
     </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A330" s="15" t="str">
+        <f>LOOKUP(B330,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B330" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C330" s="15" t="str">
+        <f>LOOKUP(D330,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>OBJECTID</v>
+      </c>
+      <c r="D330" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E330" s="6">
+        <v>1</v>
+      </c>
+      <c r="F330" s="5">
+        <v>1</v>
+      </c>
+      <c r="G330" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A331" s="15" t="str">
+        <f>LOOKUP(B331,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B331" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C331" s="15" t="str">
+        <f>LOOKUP(D331,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Feature URI</v>
+      </c>
+      <c r="D331" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="E331" s="6">
+        <v>1</v>
+      </c>
+      <c r="F331" s="5">
+        <v>2</v>
+      </c>
+      <c r="G331" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A332" s="15" t="str">
+        <f>LOOKUP(B332,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B332" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C332" s="15" t="str">
+        <f>LOOKUP(D332,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Volc Vent Name</v>
+      </c>
+      <c r="D332" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="E332" s="6">
+        <v>1</v>
+      </c>
+      <c r="F332" s="5">
+        <v>3</v>
+      </c>
+      <c r="G332" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A333" s="15" t="str">
+        <f>LOOKUP(B333,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B333" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C333" s="15" t="str">
+        <f>LOOKUP(D333,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Label</v>
+      </c>
+      <c r="D333" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E333" s="6">
+        <v>1</v>
+      </c>
+      <c r="F333" s="5">
+        <v>4</v>
+      </c>
+      <c r="G333" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A334" s="15" t="str">
+        <f>LOOKUP(B334,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B334" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C334" s="15" t="str">
+        <f>LOOKUP(D334,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Map Label</v>
+      </c>
+      <c r="D334" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="E334" s="6">
+        <v>1</v>
+      </c>
+      <c r="F334" s="5">
+        <v>5</v>
+      </c>
+      <c r="G334" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A335" s="15" t="str">
+        <f>LOOKUP(B335,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B335" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C335" s="15" t="str">
+        <f>LOOKUP(D335,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Description</v>
+      </c>
+      <c r="D335" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="E335" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F335" s="5">
+        <v>6</v>
+      </c>
+      <c r="G335" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A336" s="15" t="str">
+        <f>LOOKUP(B336,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B336" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C336" s="15" t="str">
+        <f>LOOKUP(D336,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Feature Type</v>
+      </c>
+      <c r="D336" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="E336" s="6">
+        <v>1</v>
+      </c>
+      <c r="F336" s="5">
+        <v>7</v>
+      </c>
+      <c r="G336" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A337" s="15" t="str">
+        <f>LOOKUP(B337,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B337" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C337" s="15" t="str">
+        <f>LOOKUP(D337,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Volcanic Group</v>
+      </c>
+      <c r="D337" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="E337" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F337" s="5">
+        <v>8</v>
+      </c>
+      <c r="G337" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A338" s="15" t="str">
+        <f>LOOKUP(B338,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B338" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C338" s="15" t="str">
+        <f>LOOKUP(D338,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>UTM E</v>
+      </c>
+      <c r="D338" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E338" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F338" s="5">
+        <v>9</v>
+      </c>
+      <c r="G338" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A339" s="15" t="str">
+        <f>LOOKUP(B339,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B339" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C339" s="15" t="str">
+        <f>LOOKUP(D339,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>UTM N</v>
+      </c>
+      <c r="D339" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E339" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F339" s="5">
+        <v>10</v>
+      </c>
+      <c r="G339" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A340" s="15" t="str">
+        <f>LOOKUP(B340,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B340" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C340" s="15" t="str">
+        <f>LOOKUP(D340,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>UTM Datum Zone</v>
+      </c>
+      <c r="D340" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E340" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F340" s="5">
+        <v>11</v>
+      </c>
+      <c r="G340" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A341" s="15" t="str">
+        <f>LOOKUP(B341,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B341" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C341" s="15" t="str">
+        <f>LOOKUP(D341,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Latitude Degrees</v>
+      </c>
+      <c r="D341" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E341" s="6">
+        <v>1</v>
+      </c>
+      <c r="F341" s="5">
+        <v>12</v>
+      </c>
+      <c r="G341" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A342" s="15" t="str">
+        <f>LOOKUP(B342,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B342" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C342" s="15" t="str">
+        <f>LOOKUP(D342,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Longitude Degree</v>
+      </c>
+      <c r="D342" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E342" s="6">
+        <v>1</v>
+      </c>
+      <c r="F342" s="5">
+        <v>13</v>
+      </c>
+      <c r="G342" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A343" s="15" t="str">
+        <f>LOOKUP(B343,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B343" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C343" s="15" t="str">
+        <f>LOOKUP(D343,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>SRS</v>
+      </c>
+      <c r="D343" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E343" s="6">
+        <v>1</v>
+      </c>
+      <c r="F343" s="5">
+        <v>14</v>
+      </c>
+      <c r="G343" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A344" s="15" t="str">
+        <f>LOOKUP(B344,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B344" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C344" s="15" t="str">
+        <f>LOOKUP(D344,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Location Uncertainty Statement</v>
+      </c>
+      <c r="D344" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E344" s="6">
+        <v>1</v>
+      </c>
+      <c r="F344" s="5">
+        <v>15</v>
+      </c>
+      <c r="G344" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A345" s="15" t="str">
+        <f>LOOKUP(B345,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B345" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C345" s="15" t="str">
+        <f>LOOKUP(D345,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>County</v>
+      </c>
+      <c r="D345" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E345" s="6">
+        <v>1</v>
+      </c>
+      <c r="F345" s="5">
+        <v>16</v>
+      </c>
+      <c r="G345" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A346" s="15" t="str">
+        <f>LOOKUP(B346,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B346" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C346" s="15" t="str">
+        <f>LOOKUP(D346,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>State</v>
+      </c>
+      <c r="D346" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E346" s="6">
+        <v>1</v>
+      </c>
+      <c r="F346" s="5">
+        <v>17</v>
+      </c>
+      <c r="G346" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A347" s="15" t="str">
+        <f>LOOKUP(B347,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B347" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C347" s="15" t="str">
+        <f>LOOKUP(D347,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Location Keyword</v>
+      </c>
+      <c r="D347" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E347" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F347" s="5">
+        <v>18</v>
+      </c>
+      <c r="G347" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A348" s="15" t="str">
+        <f>LOOKUP(B348,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B348" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C348" s="15" t="str">
+        <f>LOOKUP(D348,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Vent Elevation</v>
+      </c>
+      <c r="D348" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="E348" s="6">
+        <v>1</v>
+      </c>
+      <c r="F348" s="5">
+        <v>19</v>
+      </c>
+      <c r="G348" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A349" s="15" t="str">
+        <f>LOOKUP(B349,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B349" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C349" s="15" t="str">
+        <f>LOOKUP(D349,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Elevation Units of Measure</v>
+      </c>
+      <c r="D349" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="E349" s="6">
+        <v>1</v>
+      </c>
+      <c r="F349" s="5">
+        <v>20</v>
+      </c>
+      <c r="G349" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A350" s="15" t="str">
+        <f>LOOKUP(B350,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B350" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C350" s="15" t="str">
+        <f>LOOKUP(D350,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Related Feature</v>
+      </c>
+      <c r="D350" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="E350" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F350" s="5">
+        <v>21</v>
+      </c>
+      <c r="G350" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A351" s="15" t="str">
+        <f>LOOKUP(B351,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B351" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C351" s="15" t="str">
+        <f>LOOKUP(D351,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Geologic History</v>
+      </c>
+      <c r="D351" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="E351" s="6">
+        <v>1</v>
+      </c>
+      <c r="F351" s="5">
+        <v>22</v>
+      </c>
+      <c r="G351" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A352" s="15" t="str">
+        <f>LOOKUP(B352,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B352" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C352" s="15" t="str">
+        <f>LOOKUP(D352,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Youngest Age</v>
+      </c>
+      <c r="D352" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="E352" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F352" s="5">
+        <v>23</v>
+      </c>
+      <c r="G352" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="353" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A353" s="15" t="str">
+        <f>LOOKUP(B353,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B353" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C353" s="15" t="str">
+        <f>LOOKUP(D353,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Oldest Age</v>
+      </c>
+      <c r="D353" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="E353" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F353" s="5">
+        <v>24</v>
+      </c>
+      <c r="G353" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="354" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A354" s="15" t="str">
+        <f>LOOKUP(B354,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B354" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C354" s="15" t="str">
+        <f>LOOKUP(D354,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Youngest Radiometric Age Ma</v>
+      </c>
+      <c r="D354" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="E354" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F354" s="5">
+        <v>25</v>
+      </c>
+      <c r="G354" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A355" s="15" t="str">
+        <f>LOOKUP(B355,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B355" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C355" s="15" t="str">
+        <f>LOOKUP(D355,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Oldest Radiometric Age Ma</v>
+      </c>
+      <c r="D355" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="E355" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F355" s="5">
+        <v>26</v>
+      </c>
+      <c r="G355" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="356" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A356" s="15" t="str">
+        <f>LOOKUP(B356,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B356" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C356" s="15" t="str">
+        <f>LOOKUP(D356,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Age Uncertainty Ma</v>
+      </c>
+      <c r="D356" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="E356" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F356" s="5">
+        <v>27</v>
+      </c>
+      <c r="G356" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A357" s="15" t="str">
+        <f>LOOKUP(B357,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B357" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C357" s="15" t="str">
+        <f>LOOKUP(D357,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Age Source</v>
+      </c>
+      <c r="D357" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="E357" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F357" s="5">
+        <v>28</v>
+      </c>
+      <c r="G357" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A358" s="15" t="str">
+        <f>LOOKUP(B358,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B358" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C358" s="15" t="str">
+        <f>LOOKUP(D358,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Geologic Unit</v>
+      </c>
+      <c r="D358" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="E358" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F358" s="5">
+        <v>29</v>
+      </c>
+      <c r="G358" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A359" s="15" t="str">
+        <f>LOOKUP(B359,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B359" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C359" s="15" t="str">
+        <f>LOOKUP(D359,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Material Composition</v>
+      </c>
+      <c r="D359" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="E359" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F359" s="5">
+        <v>30</v>
+      </c>
+      <c r="G359" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="360" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A360" s="15" t="str">
+        <f>LOOKUP(B360,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B360" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C360" s="15" t="str">
+        <f>LOOKUP(D360,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>FlowType</v>
+      </c>
+      <c r="D360" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="E360" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F360" s="5">
+        <v>31</v>
+      </c>
+      <c r="G360" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A361" s="15" t="str">
+        <f>LOOKUP(B361,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B361" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C361" s="15" t="str">
+        <f>LOOKUP(D361,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Notes</v>
+      </c>
+      <c r="D361" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E361" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F361" s="5">
+        <v>32</v>
+      </c>
+      <c r="G361" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="362" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A362" s="15" t="str">
+        <f>LOOKUP(B362,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B362" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C362" s="15" t="str">
+        <f>LOOKUP(D362,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Source</v>
+      </c>
+      <c r="D362" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E362" s="6">
+        <v>1</v>
+      </c>
+      <c r="F362" s="5">
+        <v>33</v>
+      </c>
+      <c r="G362" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="363" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A363" s="15" t="str">
+        <f>LOOKUP(B363,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Volcanic Vent Occurrence</v>
+      </c>
+      <c r="B363" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C363" s="15" t="str">
+        <f>LOOKUP(D363,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Shape</v>
+      </c>
+      <c r="D363" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="E363" s="6">
+        <v>1</v>
+      </c>
+      <c r="F363" s="5">
+        <v>34</v>
+      </c>
+      <c r="G363" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added Thermal springs content model
added Thermal springs content model
</commit_message>
<xml_diff>
--- a/Links/Attribute-DataObject/Attribute-DataObject.xlsx
+++ b/Links/Attribute-DataObject/Attribute-DataObject.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="266">
   <si>
     <t>xs:dateTime</t>
   </si>
@@ -769,18 +769,82 @@
   </si>
   <si>
     <t>class/data-object/volcanic-vent-occurrence</t>
+  </si>
+  <si>
+    <t>class/attribute/thermalspringuri</t>
+  </si>
+  <si>
+    <t>class/attribute/springname</t>
+  </si>
+  <si>
+    <t>class/attribute/otheridentifier</t>
+  </si>
+  <si>
+    <t>class/attribute/sourceuri</t>
+  </si>
+  <si>
+    <t>class/attribute/landleaseowner</t>
+  </si>
+  <si>
+    <t>class/attribute/temperature</t>
+  </si>
+  <si>
+    <t>class/attribute/temperatureunits</t>
+  </si>
+  <si>
+    <t>class/attribute/tempmeasurementprocedure</t>
+  </si>
+  <si>
+    <t>class/attribute/tempmeasurementdatetime</t>
+  </si>
+  <si>
+    <t>class/attribute/flow</t>
+  </si>
+  <si>
+    <t>class/attribute/flowunits</t>
+  </si>
+  <si>
+    <t>class/attribute/flowmeasurementprocedure</t>
+  </si>
+  <si>
+    <t>class/attribute/flowmeasurementdatetime</t>
+  </si>
+  <si>
+    <t>class/attribute/measurementsource</t>
+  </si>
+  <si>
+    <t>class/attribute/flowcontinuity</t>
+  </si>
+  <si>
+    <t>class/attribute/classification</t>
+  </si>
+  <si>
+    <t>class/attribute/relatedwaterchemistry</t>
+  </si>
+  <si>
+    <t>class/attribute/remarks</t>
+  </si>
+  <si>
+    <t>class/data-object/thermal-spring-occurrence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -874,27 +938,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -909,14 +974,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -924,7 +989,7 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -940,12 +1005,13 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
     <cellStyle name="depth" xfId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 12 3" xfId="2"/>
     <cellStyle name="Normal 12 3 2" xfId="5"/>
+    <cellStyle name="Normal 12 3 3" xfId="11"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 2 2" xfId="6"/>
     <cellStyle name="Normal 3" xfId="7"/>
@@ -5342,1202 +5408,1202 @@
         </row>
         <row r="495">
           <cell r="A495" t="str">
-            <v>class/attribute/rank</v>
+            <v>class/attribute/range</v>
           </cell>
           <cell r="C495" t="str">
-            <v>Rank</v>
+            <v>Range</v>
           </cell>
         </row>
         <row r="496">
           <cell r="A496" t="str">
-            <v>class/attribute/rechargeprocedure1</v>
+            <v>class/attribute/rank</v>
           </cell>
           <cell r="C496" t="str">
-            <v>Recharge Procedure 1</v>
+            <v>Rank</v>
           </cell>
         </row>
         <row r="497">
           <cell r="A497" t="str">
-            <v>class/attribute/rechargeprocedure2</v>
+            <v>class/attribute/rechargeprocedure1</v>
           </cell>
           <cell r="C497" t="str">
-            <v>Recharge Procedure 2</v>
+            <v>Recharge Procedure 1</v>
           </cell>
         </row>
         <row r="498">
           <cell r="A498" t="str">
-            <v>class/attribute/recordname</v>
+            <v>class/attribute/rechargeprocedure2</v>
           </cell>
           <cell r="C498" t="str">
-            <v>Record Name</v>
+            <v>Recharge Procedure 2</v>
           </cell>
         </row>
         <row r="499">
           <cell r="A499" t="str">
-            <v>class/attribute/recurrenceinterval</v>
+            <v>class/attribute/recordname</v>
           </cell>
           <cell r="C499" t="str">
-            <v>Recurrence Interval</v>
+            <v>Record Name</v>
           </cell>
         </row>
         <row r="500">
           <cell r="A500" t="str">
-            <v>class/attribute/registrant</v>
+            <v>class/attribute/recurrenceinterval</v>
           </cell>
           <cell r="C500" t="str">
-            <v>Registrant</v>
+            <v>Recurrence Interval</v>
           </cell>
         </row>
         <row r="501">
           <cell r="A501" t="str">
-            <v>class/attribute/registranturi</v>
+            <v>class/attribute/registrant</v>
           </cell>
           <cell r="C501" t="str">
-            <v>Registrant URI</v>
+            <v>Registrant</v>
           </cell>
         </row>
         <row r="502">
           <cell r="A502" t="str">
-            <v>class/attribute/relatedfault</v>
+            <v>class/attribute/registranturi</v>
           </cell>
           <cell r="C502" t="str">
-            <v>Related Fault</v>
+            <v>Registrant URI</v>
           </cell>
         </row>
         <row r="503">
           <cell r="A503" t="str">
-            <v>class/attribute/relatedfaulturi</v>
+            <v>class/attribute/relatedfault</v>
           </cell>
           <cell r="C503" t="str">
-            <v>Related Fault URI</v>
+            <v>Related Fault</v>
           </cell>
         </row>
         <row r="504">
           <cell r="A504" t="str">
-            <v>class/attribute/relatedfeature</v>
+            <v>class/attribute/relatedfaulturi</v>
           </cell>
           <cell r="C504" t="str">
-            <v>Related Feature</v>
+            <v>Related Fault URI</v>
           </cell>
         </row>
         <row r="505">
           <cell r="A505" t="str">
-            <v>class/attribute/relatedheatflowintervalsuri</v>
+            <v>class/attribute/relatedfeature</v>
           </cell>
           <cell r="C505" t="str">
-            <v>Related Heat Flow Intervals URI</v>
+            <v>Related Feature</v>
           </cell>
         </row>
         <row r="506">
           <cell r="A506" t="str">
-            <v>class/attribute/relatedresource</v>
+            <v>class/attribute/relatedheatflowintervalsuri</v>
           </cell>
           <cell r="C506" t="str">
-            <v>Related Resource</v>
+            <v>Related Heat Flow Intervals URI</v>
           </cell>
         </row>
         <row r="507">
           <cell r="A507" t="str">
-            <v>class/attribute/relatedresources</v>
+            <v>class/attribute/relatedresource</v>
           </cell>
           <cell r="C507" t="str">
-            <v>Related Resources</v>
+            <v>Related Resource</v>
           </cell>
         </row>
         <row r="508">
           <cell r="A508" t="str">
-            <v>class/attribute/relatedsampleuri</v>
+            <v>class/attribute/relatedresources</v>
           </cell>
           <cell r="C508" t="str">
-            <v>Related Sample URI</v>
+            <v>Related Resources</v>
           </cell>
         </row>
         <row r="509">
           <cell r="A509" t="str">
-            <v>class/attribute/relatedwaterchemistry</v>
+            <v>class/attribute/relatedsampleuri</v>
           </cell>
           <cell r="C509" t="str">
-            <v>Related Water Chemistry</v>
+            <v>Related Sample URI</v>
           </cell>
         </row>
         <row r="510">
           <cell r="A510" t="str">
-            <v>class/attribute/releasedate</v>
+            <v>class/attribute/relatedwaterchemistry</v>
           </cell>
           <cell r="C510" t="str">
-            <v>Release Date</v>
+            <v>Related Water Chemistry</v>
           </cell>
         </row>
         <row r="511">
           <cell r="A511" t="str">
-            <v>class/attribute/remarks</v>
+            <v>class/attribute/releasedate</v>
           </cell>
           <cell r="C511" t="str">
-            <v>Remarks</v>
+            <v>Release Date</v>
           </cell>
         </row>
         <row r="512">
           <cell r="A512" t="str">
-            <v>class/attribute/reportingperiod</v>
+            <v>class/attribute/remarks</v>
           </cell>
           <cell r="C512" t="str">
-            <v>Reporting Period</v>
+            <v>Remarks</v>
           </cell>
         </row>
         <row r="513">
           <cell r="A513" t="str">
-            <v>class/attribute/reportyear</v>
+            <v>class/attribute/reportingperiod</v>
           </cell>
           <cell r="C513" t="str">
-            <v>Report Year</v>
+            <v>Reporting Period</v>
           </cell>
         </row>
         <row r="514">
           <cell r="A514" t="str">
-            <v>class/attribute/representativeageuri</v>
+            <v>class/attribute/reportyear</v>
           </cell>
           <cell r="C514" t="str">
-            <v>Representative Age URI</v>
+            <v>Report Year</v>
           </cell>
         </row>
         <row r="515">
           <cell r="A515" t="str">
-            <v>class/attribute/representativelithologyuri</v>
+            <v>class/attribute/representativeageuri</v>
           </cell>
           <cell r="C515" t="str">
-            <v>Representative Lithology URI</v>
+            <v>Representative Age URI</v>
           </cell>
         </row>
         <row r="516">
           <cell r="A516" t="str">
-            <v>class/attribute/reservoirfavorability</v>
+            <v>class/attribute/representativelithologyuri</v>
           </cell>
           <cell r="C516" t="str">
-            <v>Reservoir Favorability</v>
+            <v>Representative Lithology URI</v>
           </cell>
         </row>
         <row r="517">
           <cell r="A517" t="str">
-            <v>class/attribute/reservoirfavorabilitymethodology</v>
+            <v>class/attribute/reservoirfavorability</v>
           </cell>
           <cell r="C517" t="str">
-            <v>Reservoir Favorability Methodology</v>
+            <v>Reservoir Favorability</v>
           </cell>
         </row>
         <row r="518">
           <cell r="A518" t="str">
-            <v>class/attribute/reservoirfavorabilityuncertainty</v>
+            <v>class/attribute/reservoirfavorabilitymethodology</v>
           </cell>
           <cell r="C518" t="str">
-            <v>Reservoir Favorability Uncertainty</v>
+            <v>Reservoir Favorability Methodology</v>
           </cell>
         </row>
         <row r="519">
           <cell r="A519" t="str">
-            <v>class/attribute/reservoirname</v>
+            <v>class/attribute/reservoirfavorabilityuncertainty</v>
           </cell>
           <cell r="C519" t="str">
-            <v xml:space="preserve">Reservoir Name </v>
+            <v>Reservoir Favorability Uncertainty</v>
           </cell>
         </row>
         <row r="520">
           <cell r="A520" t="str">
-            <v>class/attribute/reservoiruri</v>
+            <v>class/attribute/reservoirname</v>
           </cell>
           <cell r="C520" t="str">
-            <v>Reservoir URI</v>
+            <v xml:space="preserve">Reservoir Name </v>
           </cell>
         </row>
         <row r="521">
           <cell r="A521" t="str">
-            <v>class/attribute/resistivitymud</v>
+            <v>class/attribute/reservoiruri</v>
           </cell>
           <cell r="C521" t="str">
-            <v>Mud Resistivity</v>
+            <v>Reservoir URI</v>
           </cell>
         </row>
         <row r="522">
           <cell r="A522" t="str">
-            <v>class/attribute/resistivitywater-ohm-m</v>
+            <v>class/attribute/resistivitymud</v>
           </cell>
           <cell r="C522" t="str">
-            <v>Water Resistivity ohm/m</v>
+            <v>Mud Resistivity</v>
           </cell>
         </row>
         <row r="523">
           <cell r="A523" t="str">
-            <v>class/attribute/resourcetype</v>
+            <v>class/attribute/resistivitywater-ohm-m</v>
           </cell>
           <cell r="C523" t="str">
-            <v>Resource Type</v>
+            <v>Water Resistivity ohm/m</v>
           </cell>
         </row>
         <row r="524">
           <cell r="A524" t="str">
-            <v>class/attribute/result</v>
+            <v>class/attribute/resourcetype</v>
           </cell>
           <cell r="C524" t="str">
-            <v>Result</v>
+            <v>Resource Type</v>
           </cell>
         </row>
         <row r="525">
           <cell r="A525" t="str">
-            <v>class/attribute/rge</v>
+            <v>class/attribute/result</v>
           </cell>
           <cell r="C525" t="str">
-            <v>RGE</v>
+            <v>Result</v>
           </cell>
         </row>
         <row r="526">
           <cell r="A526" t="str">
-            <v>class/attribute/rockname</v>
+            <v>class/attribute/rge</v>
           </cell>
           <cell r="C526" t="str">
-            <v>Rock Name</v>
+            <v>RGE</v>
           </cell>
         </row>
         <row r="527">
           <cell r="A527" t="str">
-            <v>class/attribute/rocktype</v>
+            <v>class/attribute/rockname</v>
           </cell>
           <cell r="C527" t="str">
-            <v>Rock Type</v>
+            <v>Rock Name</v>
           </cell>
         </row>
         <row r="528">
           <cell r="A528" t="str">
-            <v>class/attribute/salinity</v>
+            <v>class/attribute/rocktype</v>
           </cell>
           <cell r="C528" t="str">
-            <v>Salinity</v>
+            <v>Rock Type</v>
           </cell>
         </row>
         <row r="529">
           <cell r="A529" t="str">
-            <v>class/attribute/samplecollectiondate</v>
+            <v>class/attribute/salinity</v>
           </cell>
           <cell r="C529" t="str">
-            <v>Sample Collection Date</v>
+            <v>Salinity</v>
           </cell>
         </row>
         <row r="530">
           <cell r="A530" t="str">
-            <v>class/attribute/samplecollectionmethod</v>
+            <v>class/attribute/samplecollectiondate</v>
           </cell>
           <cell r="C530" t="str">
-            <v>Sample Collection Method</v>
+            <v>Sample Collection Date</v>
           </cell>
         </row>
         <row r="531">
           <cell r="A531" t="str">
-            <v>class/attribute/samplecureduration</v>
+            <v>class/attribute/samplecollectionmethod</v>
           </cell>
           <cell r="C531" t="str">
-            <v>Sample Cure Duration</v>
+            <v>Sample Collection Method</v>
           </cell>
         </row>
         <row r="532">
           <cell r="A532" t="str">
-            <v>class/attribute/sampledensity</v>
+            <v>class/attribute/samplecureduration</v>
           </cell>
           <cell r="C532" t="str">
-            <v>Sample Density</v>
+            <v>Sample Cure Duration</v>
           </cell>
         </row>
         <row r="533">
           <cell r="A533" t="str">
-            <v>class/attribute/sampledensity-g-cc</v>
+            <v>class/attribute/sampledensity</v>
           </cell>
           <cell r="C533" t="str">
-            <v>Sample Density g-cc</v>
+            <v>Sample Density</v>
           </cell>
         </row>
         <row r="534">
           <cell r="A534" t="str">
-            <v>class/attribute/sampledensityunits</v>
+            <v>class/attribute/sampledensity-g-cc</v>
           </cell>
           <cell r="C534" t="str">
-            <v>Sample Density Units</v>
+            <v>Sample Density g-cc</v>
           </cell>
         </row>
         <row r="535">
           <cell r="A535" t="str">
-            <v>class/attribute/sampledepth</v>
+            <v>class/attribute/sampledensityunits</v>
           </cell>
           <cell r="C535" t="str">
-            <v>Sample Depth</v>
+            <v>Sample Density Units</v>
           </cell>
         </row>
         <row r="536">
           <cell r="A536" t="str">
-            <v>class/attribute/sampledepth-m</v>
+            <v>class/attribute/sampledepth</v>
           </cell>
           <cell r="C536" t="str">
-            <v>Sample Depth meters</v>
+            <v>Sample Depth</v>
           </cell>
         </row>
         <row r="537">
           <cell r="A537" t="str">
-            <v>class/attribute/sampledfeatureagelabel</v>
+            <v>class/attribute/sampledepth-m</v>
           </cell>
           <cell r="C537" t="str">
-            <v>Sampled Feature Age Label</v>
+            <v>Sample Depth meters</v>
           </cell>
         </row>
         <row r="538">
           <cell r="A538" t="str">
-            <v>class/attribute/sampledfeaturemaxage-ma</v>
+            <v>class/attribute/sampledfeatureagelabel</v>
           </cell>
           <cell r="C538" t="str">
-            <v>Sampled Feature Max Age Ma</v>
+            <v>Sampled Feature Age Label</v>
           </cell>
         </row>
         <row r="539">
           <cell r="A539" t="str">
-            <v>class/attribute/sampledfeatureminage-ma</v>
+            <v>class/attribute/sampledfeaturemaxage-ma</v>
           </cell>
           <cell r="C539" t="str">
-            <v>Sampled Feature Min Age Ma</v>
+            <v>Sampled Feature Max Age Ma</v>
           </cell>
         </row>
         <row r="540">
           <cell r="A540" t="str">
-            <v>class/attribute/sampledgeologicunit</v>
+            <v>class/attribute/sampledfeatureminage-ma</v>
           </cell>
           <cell r="C540" t="str">
-            <v>Sampled Geologic Unit</v>
+            <v>Sampled Feature Min Age Ma</v>
           </cell>
         </row>
         <row r="541">
           <cell r="A541" t="str">
-            <v>class/attribute/sampledgeologicunitage</v>
+            <v>class/attribute/sampledgeologicunit</v>
           </cell>
           <cell r="C541" t="str">
-            <v>Sampled Geologic Unit Age</v>
+            <v>Sampled Geologic Unit</v>
           </cell>
         </row>
         <row r="542">
           <cell r="A542" t="str">
-            <v>class/attribute/sampledimensionsheight</v>
+            <v>class/attribute/sampledgeologicunitage</v>
           </cell>
           <cell r="C542" t="str">
-            <v>Sample Dimensions Height</v>
+            <v>Sampled Geologic Unit Age</v>
           </cell>
         </row>
         <row r="543">
           <cell r="A543" t="str">
-            <v>class/attribute/sampledimensionslength</v>
+            <v>class/attribute/sampledimensionsheight</v>
           </cell>
           <cell r="C543" t="str">
-            <v>Sample Dimensions Length</v>
+            <v>Sample Dimensions Height</v>
           </cell>
         </row>
         <row r="544">
           <cell r="A544" t="str">
-            <v>class/attribute/sampledimensionsunits</v>
+            <v>class/attribute/sampledimensionslength</v>
           </cell>
           <cell r="C544" t="str">
-            <v>Sample Dimensions Units</v>
+            <v>Sample Dimensions Length</v>
           </cell>
         </row>
         <row r="545">
           <cell r="A545" t="str">
-            <v>class/attribute/sampledimensionswidth</v>
+            <v>class/attribute/sampledimensionsunits</v>
           </cell>
           <cell r="C545" t="str">
-            <v>Sample Dimensions Width</v>
+            <v>Sample Dimensions Units</v>
           </cell>
         </row>
         <row r="546">
           <cell r="A546" t="str">
-            <v>class/attribute/samplemass-kg</v>
+            <v>class/attribute/sampledimensionswidth</v>
           </cell>
           <cell r="C546" t="str">
-            <v>Sample Mass kg</v>
+            <v>Sample Dimensions Width</v>
           </cell>
         </row>
         <row r="547">
           <cell r="A547" t="str">
-            <v>class/attribute/samplemeasurementdate</v>
+            <v>class/attribute/samplemass-kg</v>
           </cell>
           <cell r="C547" t="str">
-            <v>Sample Measurement Date</v>
+            <v>Sample Mass kg</v>
           </cell>
         </row>
         <row r="548">
           <cell r="A548" t="str">
-            <v>class/attribute/sampleshape</v>
+            <v>class/attribute/samplemeasurementdate</v>
           </cell>
           <cell r="C548" t="str">
-            <v>Sample Shape</v>
+            <v>Sample Measurement Date</v>
           </cell>
         </row>
         <row r="549">
           <cell r="A549" t="str">
-            <v>class/attribute/sampletemperature</v>
+            <v>class/attribute/sampleshape</v>
           </cell>
           <cell r="C549" t="str">
-            <v>Sample Temperature</v>
+            <v>Sample Shape</v>
           </cell>
         </row>
         <row r="550">
           <cell r="A550" t="str">
-            <v>class/attribute/sampletemperatureunits</v>
+            <v>class/attribute/sampletemperature</v>
           </cell>
           <cell r="C550" t="str">
-            <v>Sample Temperature Units</v>
+            <v>Sample Temperature</v>
           </cell>
         </row>
         <row r="551">
           <cell r="A551" t="str">
-            <v>class/attribute/sampletype</v>
+            <v>class/attribute/sampletemperatureunits</v>
           </cell>
           <cell r="C551" t="str">
-            <v>Sample Type</v>
+            <v>Sample Temperature Units</v>
           </cell>
         </row>
         <row r="552">
           <cell r="A552" t="str">
-            <v>class/attribute/samplingfeaturename</v>
+            <v>class/attribute/sampletype</v>
           </cell>
           <cell r="C552" t="str">
-            <v>Sampling Feature Name</v>
+            <v>Sample Type</v>
           </cell>
         </row>
         <row r="553">
           <cell r="A553" t="str">
-            <v>class/attribute/samplingfeaturetype</v>
+            <v>class/attribute/samplingfeaturename</v>
           </cell>
           <cell r="C553" t="str">
-            <v>Sampling Feature Type</v>
+            <v>Sampling Feature Name</v>
           </cell>
         </row>
         <row r="554">
           <cell r="A554" t="str">
-            <v>class/attribute/samplingfeatureuri</v>
+            <v>class/attribute/samplingfeaturetype</v>
           </cell>
           <cell r="C554" t="str">
-            <v>Sampling Feature URI</v>
+            <v>Sampling Feature Type</v>
           </cell>
         </row>
         <row r="555">
           <cell r="A555" t="str">
-            <v>class/attribute/saturatedsampleconductivity</v>
+            <v>class/attribute/samplingfeatureuri</v>
           </cell>
           <cell r="C555" t="str">
-            <v>Saturated Sample Conductivity</v>
+            <v>Sampling Feature URI</v>
           </cell>
         </row>
         <row r="556">
           <cell r="A556" t="str">
-            <v>class/attribute/saturationfluid</v>
+            <v>class/attribute/saturatedsampleconductivity</v>
           </cell>
           <cell r="C556" t="str">
-            <v>Saturation Fluid</v>
+            <v>Saturated Sample Conductivity</v>
           </cell>
         </row>
         <row r="557">
           <cell r="A557" t="str">
-            <v>class/attribute/scannedfileurl</v>
+            <v>class/attribute/saturationfluid</v>
           </cell>
           <cell r="C557" t="str">
-            <v>ScannedFileURL</v>
+            <v>Saturation Fluid</v>
           </cell>
         </row>
         <row r="558">
           <cell r="A558" t="str">
-            <v>class/attribute/se-conductivity</v>
+            <v>class/attribute/scannedfileurl</v>
           </cell>
           <cell r="C558" t="str">
-            <v>Standard Error Conductivity</v>
+            <v>ScannedFileURL</v>
           </cell>
         </row>
         <row r="559">
           <cell r="A559" t="str">
-            <v>class/attribute/se-correctedgradient</v>
+            <v>class/attribute/se-conductivity</v>
           </cell>
           <cell r="C559" t="str">
-            <v>Standard Error Corrected Gradient</v>
+            <v>Standard Error Conductivity</v>
           </cell>
         </row>
         <row r="560">
           <cell r="A560" t="str">
-            <v>class/attribute/se-correctedheatflow</v>
+            <v>class/attribute/se-correctedgradient</v>
           </cell>
           <cell r="C560" t="str">
-            <v>Standard Error Corrected HeatFlow</v>
+            <v>Standard Error Corrected Gradient</v>
           </cell>
         </row>
         <row r="561">
           <cell r="A561" t="str">
-            <v>class/attribute/section-</v>
+            <v>class/attribute/se-correctedheatflow</v>
           </cell>
           <cell r="C561" t="str">
-            <v xml:space="preserve">Section </v>
+            <v>Standard Error Corrected HeatFlow</v>
           </cell>
         </row>
         <row r="562">
           <cell r="A562" t="str">
-            <v>class/attribute/sectionpart</v>
+            <v>class/attribute/section-</v>
           </cell>
           <cell r="C562" t="str">
-            <v>Section Part</v>
+            <v xml:space="preserve">Section </v>
           </cell>
         </row>
         <row r="563">
           <cell r="A563" t="str">
-            <v>class/attribute/seisometernetwork</v>
+            <v>class/attribute/sectionpart</v>
           </cell>
           <cell r="C563" t="str">
-            <v>Seisometer Network</v>
+            <v>Section Part</v>
           </cell>
         </row>
         <row r="564">
           <cell r="A564" t="str">
-            <v>class/attribute/se-uncorrectedgradient</v>
+            <v>class/attribute/seisometernetwork</v>
           </cell>
           <cell r="C564" t="str">
-            <v>Standard Error Uncorrected Gradient</v>
+            <v>Seisometer Network</v>
           </cell>
         </row>
         <row r="565">
           <cell r="A565" t="str">
-            <v>class/attribute/se-uncorrectedheatflow</v>
+            <v>class/attribute/se-uncorrectedgradient</v>
           </cell>
           <cell r="C565" t="str">
-            <v>Standard Error Uncorrected HeatFlow</v>
+            <v>Standard Error Uncorrected Gradient</v>
           </cell>
         </row>
         <row r="566">
           <cell r="A566" t="str">
-            <v>class/attribute/shape</v>
+            <v>class/attribute/se-uncorrectedheatflow</v>
           </cell>
           <cell r="C566" t="str">
-            <v>Shape</v>
+            <v>Standard Error Uncorrected HeatFlow</v>
           </cell>
         </row>
         <row r="567">
           <cell r="A567" t="str">
-            <v>class/attribute/shape-area</v>
+            <v>class/attribute/shape</v>
           </cell>
           <cell r="C567" t="str">
-            <v>Shape Area</v>
+            <v>Shape</v>
           </cell>
         </row>
         <row r="568">
           <cell r="A568" t="str">
-            <v>class/attribute/shape-length</v>
+            <v>class/attribute/shape-area</v>
           </cell>
           <cell r="C568" t="str">
-            <v>Shape Length</v>
+            <v>Shape Area</v>
           </cell>
         </row>
         <row r="569">
           <cell r="A569" t="str">
-            <v>class/attribute/shutinpressuremethod</v>
+            <v>class/attribute/shape-length</v>
           </cell>
           <cell r="C569" t="str">
-            <v>Shut In Pressure Method</v>
+            <v>Shape Length</v>
           </cell>
         </row>
         <row r="570">
           <cell r="A570" t="str">
-            <v>class/attribute/siteheatflow</v>
+            <v>class/attribute/shutinpressuremethod</v>
           </cell>
           <cell r="C570" t="str">
-            <v>Site Heat Flow</v>
+            <v>Shut In Pressure Method</v>
           </cell>
         </row>
         <row r="571">
           <cell r="A571" t="str">
-            <v>class/attribute/sitelocationname</v>
+            <v>class/attribute/siteheatflow</v>
           </cell>
           <cell r="C571" t="str">
-            <v>Site Location Name</v>
+            <v>Site Heat Flow</v>
           </cell>
         </row>
         <row r="572">
           <cell r="A572" t="str">
-            <v>class/attribute/sitelocationuri</v>
+            <v>class/attribute/sitelocationname</v>
           </cell>
           <cell r="C572" t="str">
-            <v>Site Location URI</v>
+            <v>Site Location Name</v>
           </cell>
         </row>
         <row r="573">
           <cell r="A573" t="str">
-            <v>class/attribute/sitename</v>
+            <v>class/attribute/sitelocationuri</v>
           </cell>
           <cell r="C573" t="str">
-            <v>Site Name</v>
+            <v>Site Location URI</v>
           </cell>
         </row>
         <row r="574">
           <cell r="A574" t="str">
-            <v>class/attribute/sitevaluemethod</v>
+            <v>class/attribute/sitename</v>
           </cell>
           <cell r="C574" t="str">
-            <v>Site Value Method</v>
+            <v>Site Name</v>
           </cell>
         </row>
         <row r="575">
           <cell r="A575" t="str">
-            <v>class/attribute/slipaccumulationinterval</v>
+            <v>class/attribute/sitevaluemethod</v>
           </cell>
           <cell r="C575" t="str">
-            <v>Slip Accumulation Interval</v>
+            <v>Site Value Method</v>
           </cell>
         </row>
         <row r="576">
           <cell r="A576" t="str">
-            <v>class/attribute/sliprate</v>
+            <v>class/attribute/slipaccumulationinterval</v>
           </cell>
           <cell r="C576" t="str">
-            <v>Slip Rate</v>
+            <v>Slip Accumulation Interval</v>
           </cell>
         </row>
         <row r="577">
           <cell r="A577" t="str">
-            <v>class/attribute/source</v>
+            <v>class/attribute/sliprate</v>
           </cell>
           <cell r="C577" t="str">
-            <v>Source</v>
+            <v>Slip Rate</v>
           </cell>
         </row>
         <row r="578">
           <cell r="A578" t="str">
-            <v>class/attribute/sourcecitation</v>
+            <v>class/attribute/source</v>
           </cell>
           <cell r="C578" t="str">
-            <v>Source Citation</v>
+            <v>Source</v>
           </cell>
         </row>
         <row r="579">
           <cell r="A579" t="str">
-            <v>class/attribute/sourcecitationuri</v>
+            <v>class/attribute/sourcecitation</v>
           </cell>
           <cell r="C579" t="str">
-            <v>Source Citation URI</v>
+            <v>Source Citation</v>
           </cell>
         </row>
         <row r="580">
           <cell r="A580" t="str">
-            <v>class/attribute/sourceuri</v>
+            <v>class/attribute/sourcecitationuri</v>
           </cell>
           <cell r="C580" t="str">
-            <v>Source URI</v>
+            <v>Source Citation URI</v>
           </cell>
         </row>
         <row r="581">
           <cell r="A581" t="str">
-            <v>class/attribute/spacingavg-ft</v>
+            <v>class/attribute/sourceuri</v>
           </cell>
           <cell r="C581" t="str">
-            <v>Spacing Avg ft</v>
+            <v>Source URI</v>
           </cell>
         </row>
         <row r="582">
           <cell r="A582" t="str">
-            <v>class/attribute/specificationuri</v>
+            <v>class/attribute/spacingavg-ft</v>
           </cell>
           <cell r="C582" t="str">
-            <v>Specification URI</v>
+            <v>Spacing Avg ft</v>
           </cell>
         </row>
         <row r="583">
           <cell r="A583" t="str">
-            <v>class/attribute/specification-uri</v>
+            <v>class/attribute/specificationuri</v>
           </cell>
           <cell r="C583" t="str">
-            <v>specification  uri</v>
+            <v>Specification URI</v>
           </cell>
         </row>
         <row r="584">
           <cell r="A584" t="str">
-            <v>class/attribute/specificheat</v>
+            <v>class/attribute/specification-uri</v>
           </cell>
           <cell r="C584" t="str">
-            <v>Specific Heat</v>
+            <v>specification  uri</v>
           </cell>
         </row>
         <row r="585">
           <cell r="A585" t="str">
-            <v>class/attribute/specificheat-kjkgc</v>
+            <v>class/attribute/specificheat</v>
           </cell>
           <cell r="C585" t="str">
-            <v>Specific Heat kJkgC</v>
+            <v>Specific Heat</v>
           </cell>
         </row>
         <row r="586">
           <cell r="A586" t="str">
-            <v>class/attribute/specificheatunits</v>
+            <v>class/attribute/specificheat-kjkgc</v>
           </cell>
           <cell r="C586" t="str">
-            <v>Specific Heat Units</v>
+            <v>Specific Heat kJkgC</v>
           </cell>
         </row>
         <row r="587">
           <cell r="A587" t="str">
-            <v>class/attribute/specificstorage</v>
+            <v>class/attribute/specificheatunits</v>
           </cell>
           <cell r="C587" t="str">
-            <v>Specific Storage</v>
+            <v>Specific Heat Units</v>
           </cell>
         </row>
         <row r="588">
           <cell r="A588" t="str">
-            <v>class/attribute/specificyield-percent</v>
+            <v>class/attribute/specificstorage</v>
           </cell>
           <cell r="C588" t="str">
-            <v>SpecificYield percent</v>
+            <v>Specific Storage</v>
           </cell>
         </row>
         <row r="589">
           <cell r="A589" t="str">
-            <v>class/attribute/specimencollectiondate</v>
+            <v>class/attribute/specificyield-percent</v>
           </cell>
           <cell r="C589" t="str">
-            <v>Specimen Collection Date</v>
+            <v>SpecificYield percent</v>
           </cell>
         </row>
         <row r="590">
           <cell r="A590" t="str">
-            <v>class/attribute/specimencollectionmethod</v>
+            <v>class/attribute/specimencollectiondate</v>
           </cell>
           <cell r="C590" t="str">
-            <v>Specimen Collection Method</v>
+            <v>Specimen Collection Date</v>
           </cell>
         </row>
         <row r="591">
           <cell r="A591" t="str">
-            <v>class/attribute/specimencollector</v>
+            <v>class/attribute/specimencollectionmethod</v>
           </cell>
           <cell r="C591" t="str">
-            <v>Specimen Collector</v>
+            <v>Specimen Collection Method</v>
           </cell>
         </row>
         <row r="592">
           <cell r="A592" t="str">
-            <v>class/attribute/specimencollectoruri</v>
+            <v>class/attribute/specimencollector</v>
           </cell>
           <cell r="C592" t="str">
-            <v>Specimen Collector URI</v>
+            <v>Specimen Collector</v>
           </cell>
         </row>
         <row r="593">
           <cell r="A593" t="str">
-            <v>class/attribute/specimencuration</v>
+            <v>class/attribute/specimencollectoruri</v>
           </cell>
           <cell r="C593" t="str">
-            <v>Specimen Curation</v>
+            <v>Specimen Collector URI</v>
           </cell>
         </row>
         <row r="594">
           <cell r="A594" t="str">
-            <v>class/attribute/specimendescription</v>
+            <v>class/attribute/specimencuration</v>
           </cell>
           <cell r="C594" t="str">
-            <v>Specimen Description</v>
+            <v>Specimen Curation</v>
           </cell>
         </row>
         <row r="595">
           <cell r="A595" t="str">
-            <v>class/attribute/specimenid</v>
+            <v>class/attribute/specimendescription</v>
           </cell>
           <cell r="C595" t="str">
-            <v>Specimen ID</v>
+            <v>Specimen Description</v>
           </cell>
         </row>
         <row r="596">
           <cell r="A596" t="str">
-            <v>class/attribute/specimenlabel</v>
+            <v>class/attribute/specimenid</v>
           </cell>
           <cell r="C596" t="str">
-            <v>Specimen Label</v>
+            <v>Specimen ID</v>
           </cell>
         </row>
         <row r="597">
           <cell r="A597" t="str">
-            <v>class/attribute/specimenmass-kg</v>
+            <v>class/attribute/specimenlabel</v>
           </cell>
           <cell r="C597" t="str">
-            <v>Specimen Mass kg</v>
+            <v>Specimen Label</v>
           </cell>
         </row>
         <row r="598">
           <cell r="A598" t="str">
-            <v>class/attribute/specimentype</v>
+            <v>class/attribute/specimenmass-kg</v>
           </cell>
           <cell r="C598" t="str">
-            <v>SpecimenType</v>
+            <v>Specimen Mass kg</v>
           </cell>
         </row>
         <row r="599">
           <cell r="A599" t="str">
-            <v>class/attribute/specimenuri</v>
+            <v>class/attribute/specimentype</v>
           </cell>
           <cell r="C599" t="str">
-            <v>Specimen URI</v>
+            <v>SpecimenType</v>
           </cell>
         </row>
         <row r="600">
           <cell r="A600" t="str">
-            <v>class/attribute/springname</v>
+            <v>class/attribute/specimenuri</v>
           </cell>
           <cell r="C600" t="str">
-            <v>Spring Name</v>
+            <v>Specimen URI</v>
           </cell>
         </row>
         <row r="601">
           <cell r="A601" t="str">
-            <v>class/attribute/spuddate</v>
+            <v>class/attribute/springname</v>
           </cell>
           <cell r="C601" t="str">
-            <v>Spud Date</v>
+            <v>Spring Name</v>
           </cell>
         </row>
         <row r="602">
           <cell r="A602" t="str">
-            <v>class/attribute/srs</v>
+            <v>class/attribute/spuddate</v>
           </cell>
           <cell r="C602" t="str">
-            <v>SRS</v>
+            <v>Spud Date</v>
           </cell>
         </row>
         <row r="603">
           <cell r="A603" t="str">
-            <v>class/attribute/standarddeviation</v>
+            <v>class/attribute/srs</v>
           </cell>
           <cell r="C603" t="str">
-            <v>Standard Deviation</v>
+            <v>SRS</v>
           </cell>
         </row>
         <row r="604">
           <cell r="A604" t="str">
-            <v>class/attribute/standardmagnitudeerror</v>
+            <v>class/attribute/standarddeviation</v>
           </cell>
           <cell r="C604" t="str">
-            <v>Standard Magnitude Error</v>
+            <v>Standard Deviation</v>
           </cell>
         </row>
         <row r="605">
           <cell r="A605" t="str">
-            <v>class/attribute/startreportinterval</v>
+            <v>class/attribute/standardmagnitudeerror</v>
           </cell>
           <cell r="C605" t="str">
-            <v>Start Report Interval</v>
+            <v>Standard Magnitude Error</v>
           </cell>
         </row>
         <row r="606">
           <cell r="A606" t="str">
-            <v>class/attribute/state</v>
+            <v>class/attribute/startreportinterval</v>
           </cell>
           <cell r="C606" t="str">
-            <v>State</v>
+            <v>Start Report Interval</v>
           </cell>
         </row>
         <row r="607">
           <cell r="A607" t="str">
-            <v>class/attribute/stationidentifier</v>
+            <v>class/attribute/state</v>
           </cell>
           <cell r="C607" t="str">
-            <v>Station Identifier</v>
+            <v>State</v>
           </cell>
         </row>
         <row r="608">
           <cell r="A608" t="str">
-            <v>class/attribute/stationname</v>
+            <v>class/attribute/stationidentifier</v>
           </cell>
           <cell r="C608" t="str">
-            <v>Station Name</v>
+            <v>Station Identifier</v>
           </cell>
         </row>
         <row r="609">
           <cell r="A609" t="str">
-            <v>class/attribute/statisticalprocedure</v>
+            <v>class/attribute/stationname</v>
           </cell>
           <cell r="C609" t="str">
-            <v>Statistical procedure</v>
+            <v>Station Name</v>
           </cell>
         </row>
         <row r="610">
           <cell r="A610" t="str">
-            <v>class/attribute/status</v>
+            <v>class/attribute/statisticalprocedure</v>
           </cell>
           <cell r="C610" t="str">
-            <v>Status</v>
+            <v>Statistical procedure</v>
           </cell>
         </row>
         <row r="611">
           <cell r="A611" t="str">
-            <v>class/attribute/statusdate</v>
+            <v>class/attribute/status</v>
           </cell>
           <cell r="C611" t="str">
-            <v>Status Date</v>
+            <v>Status</v>
           </cell>
         </row>
         <row r="612">
           <cell r="A612" t="str">
-            <v>class/attribute/stimulation</v>
+            <v>class/attribute/statusdate</v>
           </cell>
           <cell r="C612" t="str">
-            <v>Stimulation</v>
+            <v>Status Date</v>
           </cell>
         </row>
         <row r="613">
           <cell r="A613" t="str">
-            <v>class/attribute/surfacetemperature</v>
+            <v>class/attribute/stimulation</v>
           </cell>
           <cell r="C613" t="str">
-            <v>Surface Temperature</v>
+            <v>Stimulation</v>
           </cell>
         </row>
         <row r="614">
           <cell r="A614" t="str">
-            <v>class/attribute/symbol</v>
+            <v>class/attribute/surfacetemperature</v>
           </cell>
           <cell r="C614" t="str">
-            <v>Symbol</v>
+            <v>Surface Temperature</v>
           </cell>
         </row>
         <row r="615">
           <cell r="A615" t="str">
-            <v>class/attribute/systemtype</v>
+            <v>class/attribute/symbol</v>
           </cell>
           <cell r="C615" t="str">
-            <v>System Type</v>
+            <v>Symbol</v>
           </cell>
         </row>
         <row r="616">
           <cell r="A616" t="str">
-            <v>class/attribute/targetfeatureuri</v>
+            <v>class/attribute/systemtype</v>
           </cell>
           <cell r="C616" t="str">
-            <v>Target Feature URI</v>
+            <v>System Type</v>
           </cell>
         </row>
         <row r="617">
           <cell r="A617" t="str">
-            <v>class/attribute/targetformation</v>
+            <v>class/attribute/targetfeatureuri</v>
           </cell>
           <cell r="C617" t="str">
-            <v>Target Formation</v>
+            <v>Target Feature URI</v>
           </cell>
         </row>
         <row r="618">
           <cell r="A618" t="str">
-            <v>class/attribute/targetrockname</v>
+            <v>class/attribute/targetformation</v>
           </cell>
           <cell r="C618" t="str">
-            <v>Target Rock Name</v>
+            <v>Target Formation</v>
           </cell>
         </row>
         <row r="619">
           <cell r="A619" t="str">
-            <v>class/attribute/targetrockvolume-m3</v>
+            <v>class/attribute/targetrockname</v>
           </cell>
           <cell r="C619" t="str">
-            <v>Target Rock Volume m3</v>
+            <v>Target Rock Name</v>
           </cell>
         </row>
         <row r="620">
           <cell r="A620" t="str">
-            <v>class/attribute/tectonicprovince</v>
+            <v>class/attribute/targetrockvolume-m3</v>
           </cell>
           <cell r="C620" t="str">
-            <v>Tectonic Province</v>
+            <v>Target Rock Volume m3</v>
           </cell>
         </row>
         <row r="621">
           <cell r="A621" t="str">
-            <v>class/attribute/temperature</v>
+            <v>class/attribute/tectonicprovince</v>
           </cell>
           <cell r="C621" t="str">
-            <v>Temperature</v>
+            <v>Tectonic Province</v>
           </cell>
         </row>
         <row r="622">
           <cell r="A622" t="str">
-            <v>class/attribute/temperaturecorrection</v>
+            <v>class/attribute/temperature</v>
           </cell>
           <cell r="C622" t="str">
-            <v>Temperature Correction</v>
+            <v>Temperature</v>
           </cell>
         </row>
         <row r="623">
           <cell r="A623" t="str">
-            <v>class/attribute/temperature-f</v>
+            <v>class/attribute/temperaturecorrection</v>
           </cell>
           <cell r="C623" t="str">
-            <v>Temperature Fahrenheit</v>
+            <v>Temperature Correction</v>
           </cell>
         </row>
         <row r="624">
           <cell r="A624" t="str">
-            <v>class/attribute/temperatureflowing</v>
+            <v>class/attribute/temperature-f</v>
           </cell>
           <cell r="C624" t="str">
-            <v>Temperature Flowing</v>
+            <v>Temperature Fahrenheit</v>
           </cell>
         </row>
         <row r="625">
           <cell r="A625" t="str">
-            <v>class/attribute/temperaturemax-c</v>
+            <v>class/attribute/temperatureflowing</v>
           </cell>
           <cell r="C625" t="str">
-            <v>Temperature Max C</v>
+            <v>Temperature Flowing</v>
           </cell>
         </row>
         <row r="626">
           <cell r="A626" t="str">
-            <v>class/attribute/temperaturemeasuretype</v>
+            <v>class/attribute/temperaturemax-c</v>
           </cell>
           <cell r="C626" t="str">
-            <v>Temperature Measure Type</v>
+            <v>Temperature Max C</v>
           </cell>
         </row>
         <row r="627">
           <cell r="A627" t="str">
-            <v>class/attribute/temperaturemin-c</v>
+            <v>class/attribute/temperaturemeasuretype</v>
           </cell>
           <cell r="C627" t="str">
-            <v>Temperature Min C</v>
+            <v>Temperature Measure Type</v>
           </cell>
         </row>
         <row r="628">
           <cell r="A628" t="str">
-            <v>class/attribute/temperatureunits</v>
+            <v>class/attribute/temperaturemin-c</v>
           </cell>
           <cell r="C628" t="str">
-            <v>Temperature Units</v>
+            <v>Temperature Min C</v>
           </cell>
         </row>
         <row r="629">
           <cell r="A629" t="str">
-            <v>class/attribute/tempmeasurementdatetime</v>
+            <v>class/attribute/temperatureunits</v>
           </cell>
           <cell r="C629" t="str">
-            <v>Temp Measurement Date Time</v>
+            <v>Temperature Units</v>
           </cell>
         </row>
         <row r="630">
           <cell r="A630" t="str">
-            <v>class/attribute/tempmeasurementprocedure</v>
+            <v>class/attribute/tempmeasurementdatetime</v>
           </cell>
           <cell r="C630" t="str">
-            <v>Temp Measurement Procedure</v>
+            <v>Temp Measurement Date Time</v>
           </cell>
         </row>
         <row r="631">
           <cell r="A631" t="str">
-            <v>class/attribute/terraincorrection-mgal</v>
+            <v>class/attribute/tempmeasurementprocedure</v>
           </cell>
           <cell r="C631" t="str">
-            <v>Terrain Correction mgal</v>
+            <v>Temp Measurement Procedure</v>
           </cell>
         </row>
         <row r="632">
           <cell r="A632" t="str">
-            <v>class/attribute/testdatetime</v>
+            <v>class/attribute/terraincorrection-mgal</v>
           </cell>
           <cell r="C632" t="str">
-            <v>Test date time</v>
+            <v>Terrain Correction mgal</v>
           </cell>
         </row>
         <row r="633">
           <cell r="A633" t="str">
-            <v>class/attribute/testfluid</v>
+            <v>class/attribute/testdatetime</v>
           </cell>
           <cell r="C633" t="str">
-            <v>Test Fluid</v>
+            <v>Test date time</v>
           </cell>
         </row>
         <row r="634">
           <cell r="A634" t="str">
-            <v>class/attribute/testname</v>
+            <v>class/attribute/testfluid</v>
           </cell>
           <cell r="C634" t="str">
-            <v>Test Name</v>
+            <v>Test Fluid</v>
           </cell>
         </row>
         <row r="635">
           <cell r="A635" t="str">
-            <v>class/attribute/testnumber</v>
+            <v>class/attribute/testname</v>
           </cell>
           <cell r="C635" t="str">
-            <v>Test Number</v>
+            <v>Test Name</v>
           </cell>
         </row>
         <row r="636">
           <cell r="A636" t="str">
-            <v>class/attribute/testoperator</v>
+            <v>class/attribute/testnumber</v>
           </cell>
           <cell r="C636" t="str">
-            <v>Test Operator</v>
+            <v>Test Number</v>
           </cell>
         </row>
         <row r="637">
           <cell r="A637" t="str">
-            <v>class/attribute/testtype</v>
+            <v>class/attribute/testoperator</v>
           </cell>
           <cell r="C637" t="str">
-            <v>Test Type</v>
+            <v>Test Operator</v>
           </cell>
         </row>
         <row r="638">
           <cell r="A638" t="str">
-            <v>class/attribute/testtypedescription</v>
+            <v>class/attribute/testtype</v>
           </cell>
           <cell r="C638" t="str">
-            <v>Test Type Description</v>
+            <v>Test Type</v>
           </cell>
         </row>
         <row r="639">
           <cell r="A639" t="str">
-            <v>class/attribute/thermalconductivityunits</v>
+            <v>class/attribute/testtypedescription</v>
           </cell>
           <cell r="C639" t="str">
-            <v>Thermal Conductivity Units</v>
+            <v>Test Type Description</v>
           </cell>
         </row>
         <row r="640">
           <cell r="A640" t="str">
-            <v>class/attribute/thermaldiffusivity</v>
+            <v>class/attribute/thermalconductivityunits</v>
           </cell>
           <cell r="C640" t="str">
-            <v>Thermal Diffusivity</v>
+            <v>Thermal Conductivity Units</v>
           </cell>
         </row>
         <row r="641">
           <cell r="A641" t="str">
-            <v>class/attribute/thermalspringuri</v>
+            <v>class/attribute/thermaldiffusivity</v>
           </cell>
           <cell r="C641" t="str">
-            <v>Thermal Spring URI</v>
+            <v>Thermal Diffusivity</v>
           </cell>
         </row>
         <row r="642">
           <cell r="A642" t="str">
-            <v>class/attribute/timefinalshutin-min</v>
+            <v>class/attribute/thermalspringuri</v>
           </cell>
           <cell r="C642" t="str">
-            <v>Time Final Shut In min</v>
+            <v>Thermal Spring URI</v>
           </cell>
         </row>
         <row r="643">
           <cell r="A643" t="str">
-            <v>class/attribute/timeinitialshutin-min</v>
+            <v>class/attribute/timefinalshutin-min</v>
           </cell>
           <cell r="C643" t="str">
-            <v>Time Initial Shut In min</v>
+            <v>Time Final Shut In min</v>
           </cell>
         </row>
         <row r="644">
           <cell r="A644" t="str">
-            <v>class/attribute/timesincecirculation</v>
+            <v>class/attribute/timeinitialshutin-min</v>
           </cell>
           <cell r="C644" t="str">
-            <v>Time Since Circulation</v>
+            <v>Time Initial Shut In min</v>
           </cell>
         </row>
         <row r="645">
@@ -6545,518 +6611,534 @@
             <v>class/attribute/timesincecirculation</v>
           </cell>
           <cell r="C645" t="str">
-            <v xml:space="preserve">Time Since Circulation </v>
+            <v>Time Since Circulation</v>
           </cell>
         </row>
         <row r="646">
           <cell r="A646" t="str">
-            <v>class/attribute/toploggedinterval-ft</v>
+            <v>class/attribute/timesincecirculation</v>
           </cell>
           <cell r="C646" t="str">
-            <v>Top Logged Interval ft</v>
+            <v xml:space="preserve">Time Since Circulation </v>
           </cell>
         </row>
         <row r="647">
           <cell r="A647" t="str">
-            <v>class/attribute/totalmineheat-kj</v>
+            <v>class/attribute/toploggedinterval-ft</v>
           </cell>
           <cell r="C647" t="str">
-            <v>Total Mine Heat kJ</v>
+            <v>Top Logged Interval ft</v>
           </cell>
         </row>
         <row r="648">
           <cell r="A648" t="str">
-            <v>class/attribute/totalslip</v>
+            <v>class/attribute/totalmineheat-kj</v>
           </cell>
           <cell r="C648" t="str">
-            <v>Total Slip</v>
+            <v>Total Mine Heat kJ</v>
           </cell>
         </row>
         <row r="649">
           <cell r="A649" t="str">
-            <v>class/attribute/transmissivity</v>
+            <v>class/attribute/totalslip</v>
           </cell>
           <cell r="C649" t="str">
-            <v>Transmissivity</v>
+            <v>Total Slip</v>
           </cell>
         </row>
         <row r="650">
           <cell r="A650" t="str">
-            <v>class/attribute/transmissivity-units</v>
+            <v>class/attribute/township</v>
           </cell>
           <cell r="C650" t="str">
-            <v>Transmissivity units</v>
+            <v>Township</v>
           </cell>
         </row>
         <row r="651">
           <cell r="A651" t="str">
-            <v>class/attribute/trap</v>
+            <v>class/attribute/transmissivity</v>
           </cell>
           <cell r="C651" t="str">
-            <v>Trap</v>
+            <v>Transmissivity</v>
           </cell>
         </row>
         <row r="652">
           <cell r="A652" t="str">
-            <v>class/attribute/trueverticaldepth</v>
+            <v>class/attribute/transmissivity-units</v>
           </cell>
           <cell r="C652" t="str">
-            <v>True Vertical Depth</v>
+            <v>Transmissivity units</v>
           </cell>
         </row>
         <row r="653">
           <cell r="A653" t="str">
-            <v>class/attribute/twp</v>
+            <v>class/attribute/trap</v>
           </cell>
           <cell r="C653" t="str">
-            <v>TWP</v>
+            <v>Trap</v>
           </cell>
         </row>
         <row r="654">
           <cell r="A654" t="str">
-            <v>class/attribute/uncertainty</v>
+            <v>class/attribute/trueverticaldepth</v>
           </cell>
           <cell r="C654" t="str">
-            <v>uncertainty</v>
+            <v>True Vertical Depth</v>
           </cell>
         </row>
         <row r="655">
           <cell r="A655" t="str">
-            <v>class/attribute/uncertaintydensity</v>
+            <v>class/attribute/twp</v>
           </cell>
           <cell r="C655" t="str">
-            <v>UncertaintyDensity</v>
+            <v>TWP</v>
           </cell>
         </row>
         <row r="656">
           <cell r="A656" t="str">
-            <v>class/attribute/uncertainty-mgal</v>
+            <v>class/attribute/uncertainty</v>
           </cell>
           <cell r="C656" t="str">
-            <v>Uncertainty mgal</v>
+            <v>uncertainty</v>
           </cell>
         </row>
         <row r="657">
           <cell r="A657" t="str">
-            <v>class/attribute/uncertaintyspecificheat</v>
+            <v>class/attribute/uncertaintydensity</v>
           </cell>
           <cell r="C657" t="str">
-            <v>Uncertainty Specific Heat</v>
+            <v>UncertaintyDensity</v>
           </cell>
         </row>
         <row r="658">
           <cell r="A658" t="str">
-            <v>class/attribute/uncertaintytc</v>
+            <v>class/attribute/uncertainty-mgal</v>
           </cell>
           <cell r="C658" t="str">
-            <v>Uncertainty Thermal Conductivity</v>
+            <v>Uncertainty mgal</v>
           </cell>
         </row>
         <row r="659">
           <cell r="A659" t="str">
-            <v>class/attribute/uncertaintythermaldiffusivity</v>
+            <v>class/attribute/uncertaintyspecificheat</v>
           </cell>
           <cell r="C659" t="str">
-            <v>Uncertainty Thermal Diffusivity</v>
+            <v>Uncertainty Specific Heat</v>
           </cell>
         </row>
         <row r="660">
           <cell r="A660" t="str">
-            <v>class/attribute/units</v>
+            <v>class/attribute/uncertaintytc</v>
           </cell>
           <cell r="C660" t="str">
-            <v>Units Of Measure</v>
+            <v>Uncertainty Thermal Conductivity</v>
           </cell>
         </row>
         <row r="661">
           <cell r="A661" t="str">
-            <v>class/attribute/unitsofmeasure</v>
+            <v>class/attribute/uncertaintythermaldiffusivity</v>
           </cell>
           <cell r="C661" t="str">
-            <v>Units Of Measure</v>
+            <v>Uncertainty Thermal Diffusivity</v>
           </cell>
         </row>
         <row r="662">
           <cell r="A662" t="str">
-            <v>class/attribute/unitspermeability</v>
+            <v>class/attribute/units</v>
           </cell>
           <cell r="C662" t="str">
-            <v>Permeability units</v>
+            <v>Units Of Measure</v>
           </cell>
         </row>
         <row r="663">
           <cell r="A663" t="str">
-            <v>class/attribute/unitsporosity</v>
+            <v>class/attribute/unitsofmeasure</v>
           </cell>
           <cell r="C663" t="str">
-            <v>Porosity units</v>
+            <v>Units Of Measure</v>
           </cell>
         </row>
         <row r="664">
           <cell r="A664" t="str">
-            <v>class/attribute/units-pressure</v>
+            <v>class/attribute/unitspermeability</v>
           </cell>
           <cell r="C664" t="str">
-            <v>Pressure units</v>
+            <v>Permeability units</v>
           </cell>
         </row>
         <row r="665">
           <cell r="A665" t="str">
-            <v>class/attribute/unitsstorage</v>
+            <v>class/attribute/unitsporosity</v>
           </cell>
           <cell r="C665" t="str">
-            <v>Storage units</v>
+            <v>Porosity units</v>
           </cell>
         </row>
         <row r="666">
           <cell r="A666" t="str">
-            <v>class/attribute/unitstc</v>
+            <v>class/attribute/units-pressure</v>
           </cell>
           <cell r="C666" t="str">
-            <v>Thermal Conductivity Units</v>
+            <v>Pressure units</v>
           </cell>
         </row>
         <row r="667">
           <cell r="A667" t="str">
-            <v>class/attribute/units-temperature</v>
+            <v>class/attribute/unitsstorage</v>
           </cell>
           <cell r="C667" t="str">
-            <v>Temperature units</v>
+            <v>Storage units</v>
           </cell>
         </row>
         <row r="668">
           <cell r="A668" t="str">
-            <v>class/attribute/unitsthermaldiffusivity</v>
+            <v>class/attribute/unitstc</v>
           </cell>
           <cell r="C668" t="str">
-            <v>Thermal Diffusivity units</v>
+            <v>Thermal Conductivity Units</v>
           </cell>
         </row>
         <row r="669">
           <cell r="A669" t="str">
-            <v>class/attribute/updatedate</v>
+            <v>class/attribute/units-temperature</v>
           </cell>
           <cell r="C669" t="str">
-            <v>Update Date</v>
+            <v>Temperature units</v>
           </cell>
         </row>
         <row r="670">
           <cell r="A670" t="str">
-            <v>class/attribute/updatetimestamp</v>
+            <v>class/attribute/unitsthermaldiffusivity</v>
           </cell>
           <cell r="C670" t="str">
-            <v>Update Time Stamp</v>
+            <v>Thermal Diffusivity units</v>
           </cell>
         </row>
         <row r="671">
           <cell r="A671" t="str">
-            <v>class/attribute/useapplication</v>
+            <v>class/attribute/updatedate</v>
           </cell>
           <cell r="C671" t="str">
-            <v>Use Application</v>
+            <v>Update Date</v>
           </cell>
         </row>
         <row r="672">
           <cell r="A672" t="str">
-            <v>class/attribute/utmdatumzone</v>
+            <v>class/attribute/updatetimestamp</v>
           </cell>
           <cell r="C672" t="str">
-            <v>UTM Datum Zone</v>
+            <v>Update Time Stamp</v>
           </cell>
         </row>
         <row r="673">
           <cell r="A673" t="str">
-            <v>class/attribute/utm-e</v>
+            <v>class/attribute/useapplication</v>
           </cell>
           <cell r="C673" t="str">
-            <v>UTM E</v>
+            <v>Use Application</v>
           </cell>
         </row>
         <row r="674">
           <cell r="A674" t="str">
-            <v>class/attribute/utm-n</v>
+            <v>class/attribute/utmdatumzone</v>
           </cell>
           <cell r="C674" t="str">
-            <v>UTM N</v>
+            <v>UTM Datum Zone</v>
           </cell>
         </row>
         <row r="675">
           <cell r="A675" t="str">
-            <v>class/attribute/utmzone</v>
+            <v>class/attribute/utm-e</v>
           </cell>
           <cell r="C675" t="str">
-            <v>UTM Zone</v>
+            <v>UTM E</v>
           </cell>
         </row>
         <row r="676">
           <cell r="A676" t="str">
-            <v>class/attribute/ventelevation</v>
+            <v>class/attribute/utm-n</v>
           </cell>
           <cell r="C676" t="str">
-            <v>Vent Elevation</v>
+            <v>UTM N</v>
           </cell>
         </row>
         <row r="677">
           <cell r="A677" t="str">
-            <v>class/attribute/verticalconductivity-ft-day</v>
+            <v>class/attribute/utmzone</v>
           </cell>
           <cell r="C677" t="str">
-            <v>Vertical Conductivity ft day</v>
+            <v>UTM Zone</v>
           </cell>
         </row>
         <row r="678">
           <cell r="A678" t="str">
-            <v>class/attribute/verticaldatum</v>
+            <v>class/attribute/ventelevation</v>
           </cell>
           <cell r="C678" t="str">
-            <v>Vertical Datum</v>
+            <v>Vent Elevation</v>
           </cell>
         </row>
         <row r="679">
           <cell r="A679" t="str">
-            <v>class/attribute/verticalextentmax-m</v>
+            <v>class/attribute/verticalconductivity-ft-day</v>
           </cell>
           <cell r="C679" t="str">
-            <v>Vertical Extent Max m</v>
+            <v>Vertical Conductivity ft day</v>
           </cell>
         </row>
         <row r="680">
           <cell r="A680" t="str">
-            <v>class/attribute/verticalextentmin-m</v>
+            <v>class/attribute/verticaldatum</v>
           </cell>
           <cell r="C680" t="str">
-            <v>Vertical Extent Min m</v>
+            <v>Vertical Datum</v>
           </cell>
         </row>
         <row r="681">
           <cell r="A681" t="str">
-            <v>class/attribute/verticalunits</v>
+            <v>class/attribute/verticalextentmax-m</v>
           </cell>
           <cell r="C681" t="str">
-            <v>Vertical Units</v>
+            <v>Vertical Extent Max m</v>
           </cell>
         </row>
         <row r="682">
           <cell r="A682" t="str">
-            <v>class/attribute/viscosity</v>
+            <v>class/attribute/verticalextentmin-m</v>
           </cell>
           <cell r="C682" t="str">
-            <v>Viscosity</v>
+            <v>Vertical Extent Min m</v>
           </cell>
         </row>
         <row r="683">
           <cell r="A683" t="str">
-            <v>class/attribute/volcanicgroup</v>
+            <v>class/attribute/verticalunits</v>
           </cell>
           <cell r="C683" t="str">
-            <v>Volcanic Group</v>
+            <v>Vertical Units</v>
           </cell>
         </row>
         <row r="684">
           <cell r="A684" t="str">
-            <v>class/attribute/volcventname</v>
+            <v>class/attribute/viscosity</v>
           </cell>
           <cell r="C684" t="str">
-            <v>Volc Vent Name</v>
+            <v>Viscosity</v>
           </cell>
         </row>
         <row r="685">
           <cell r="A685" t="str">
-            <v>class/attribute/waterdensity-kgm3</v>
+            <v>class/attribute/volcanicgroup</v>
           </cell>
           <cell r="C685" t="str">
-            <v>Water Density  kgm3</v>
+            <v>Volcanic Group</v>
           </cell>
         </row>
         <row r="686">
           <cell r="A686" t="str">
-            <v>class/attribute/waterdensity-mgl</v>
+            <v>class/attribute/volcventname</v>
           </cell>
           <cell r="C686" t="str">
-            <v>Water Density  mgL</v>
+            <v>Volc Vent Name</v>
           </cell>
         </row>
         <row r="687">
           <cell r="A687" t="str">
-            <v>class/attribute/waterinjection-bbl</v>
+            <v>class/attribute/waterdensity-kgm3</v>
           </cell>
           <cell r="C687" t="str">
-            <v>Water Injection bbl</v>
+            <v>Water Density  kgm3</v>
           </cell>
         </row>
         <row r="688">
           <cell r="A688" t="str">
-            <v>class/attribute/watermass-kg</v>
+            <v>class/attribute/waterdensity-mgl</v>
           </cell>
           <cell r="C688" t="str">
-            <v>Water Mass kg</v>
+            <v>Water Density  mgL</v>
           </cell>
         </row>
         <row r="689">
           <cell r="A689" t="str">
-            <v>class/attribute/watersaturation-pct</v>
+            <v>class/attribute/waterinjection-bbl</v>
           </cell>
           <cell r="C689" t="str">
-            <v>Water Saturation pct</v>
+            <v>Water Injection bbl</v>
           </cell>
         </row>
         <row r="690">
           <cell r="A690" t="str">
-            <v>class/attribute/watershedname</v>
+            <v>class/attribute/watermass-kg</v>
           </cell>
           <cell r="C690" t="str">
-            <v>Watershed Name</v>
+            <v>Water Mass kg</v>
           </cell>
         </row>
         <row r="691">
           <cell r="A691" t="str">
-            <v>class/attribute/watertabletemperature</v>
+            <v>class/attribute/watersaturation-pct</v>
           </cell>
           <cell r="C691" t="str">
-            <v>Water Table Temperature</v>
+            <v>Water Saturation pct</v>
           </cell>
         </row>
         <row r="692">
           <cell r="A692" t="str">
-            <v>class/attribute/watertabletop</v>
+            <v>class/attribute/watershedname</v>
           </cell>
           <cell r="C692" t="str">
-            <v>Water Table Top</v>
+            <v>Watershed Name</v>
           </cell>
         </row>
         <row r="693">
           <cell r="A693" t="str">
-            <v>class/attribute/watertds-mgl</v>
+            <v>class/attribute/watertabletemperature</v>
           </cell>
           <cell r="C693" t="str">
-            <v>Water TDS mgl</v>
+            <v>Water Table Temperature</v>
           </cell>
         </row>
         <row r="694">
           <cell r="A694" t="str">
-            <v>class/attribute/wellborename</v>
+            <v>class/attribute/watertabletop</v>
           </cell>
           <cell r="C694" t="str">
-            <v xml:space="preserve">WellBore Name </v>
+            <v>Water Table Top</v>
           </cell>
         </row>
         <row r="695">
           <cell r="A695" t="str">
-            <v>class/attribute/wellboreshape</v>
+            <v>class/attribute/watertds-mgl</v>
           </cell>
           <cell r="C695" t="str">
-            <v>Well Bore Shape</v>
+            <v>Water TDS mgl</v>
           </cell>
         </row>
         <row r="696">
           <cell r="A696" t="str">
-            <v>class/attribute/wellboreuri</v>
+            <v>class/attribute/wellborename</v>
           </cell>
           <cell r="C696" t="str">
-            <v>WellBore URI</v>
+            <v xml:space="preserve">WellBore Name </v>
           </cell>
         </row>
         <row r="697">
           <cell r="A697" t="str">
-            <v>class/attribute/wellcount</v>
+            <v>class/attribute/wellboreshape</v>
           </cell>
           <cell r="C697" t="str">
-            <v>Well Count</v>
+            <v>Well Bore Shape</v>
           </cell>
         </row>
         <row r="698">
           <cell r="A698" t="str">
-            <v>class/attribute/welldrilldate</v>
+            <v>class/attribute/wellboreuri</v>
           </cell>
           <cell r="C698" t="str">
-            <v>Well Drill Date</v>
+            <v>WellBore URI</v>
           </cell>
         </row>
         <row r="699">
           <cell r="A699" t="str">
-            <v>class/attribute/welldrilldatetype</v>
+            <v>class/attribute/wellcount</v>
           </cell>
           <cell r="C699" t="str">
-            <v>Well Drill Date Type</v>
+            <v>Well Count</v>
           </cell>
         </row>
         <row r="700">
           <cell r="A700" t="str">
-            <v>class/attribute/wellheaderuri</v>
+            <v>class/attribute/welldrilldate</v>
           </cell>
           <cell r="C700" t="str">
-            <v>Well Header URI</v>
+            <v>Well Drill Date</v>
           </cell>
         </row>
         <row r="701">
           <cell r="A701" t="str">
-            <v>class/attribute/wellname</v>
+            <v>class/attribute/welldrilldatetype</v>
           </cell>
           <cell r="C701" t="str">
-            <v>Well Name</v>
+            <v>Well Drill Date Type</v>
           </cell>
         </row>
         <row r="702">
           <cell r="A702" t="str">
-            <v>class/attribute/welltype</v>
+            <v>class/attribute/wellheaderuri</v>
           </cell>
           <cell r="C702" t="str">
-            <v>Well Type</v>
+            <v>Well Header URI</v>
           </cell>
         </row>
         <row r="703">
           <cell r="A703" t="str">
-            <v>class/attribute/width-m</v>
+            <v>class/attribute/wellname</v>
           </cell>
           <cell r="C703" t="str">
-            <v>Width m</v>
+            <v>Well Name</v>
           </cell>
         </row>
         <row r="704">
           <cell r="A704" t="str">
-            <v>class/attribute/yearcommissioned</v>
+            <v>class/attribute/welltype</v>
           </cell>
           <cell r="C704" t="str">
-            <v>Year Commissioned</v>
+            <v>Well Type</v>
           </cell>
         </row>
         <row r="705">
           <cell r="A705" t="str">
-            <v>class/attribute/yearsinproduction</v>
+            <v>class/attribute/width-m</v>
           </cell>
           <cell r="C705" t="str">
-            <v>Years In Production</v>
+            <v>Width m</v>
           </cell>
         </row>
         <row r="706">
           <cell r="A706" t="str">
-            <v>class/attribute/youngerageuri</v>
+            <v>class/attribute/yearcommissioned</v>
           </cell>
           <cell r="C706" t="str">
-            <v>Younger Age URI</v>
+            <v>Year Commissioned</v>
           </cell>
         </row>
         <row r="707">
           <cell r="A707" t="str">
-            <v>class/attribute/youngestage</v>
+            <v>class/attribute/yearsinproduction</v>
           </cell>
           <cell r="C707" t="str">
-            <v>Youngest Age</v>
+            <v>Years In Production</v>
           </cell>
         </row>
         <row r="708">
           <cell r="A708" t="str">
-            <v>class/attribute/youngestradiometricage-ma</v>
+            <v>class/attribute/youngerageuri</v>
           </cell>
           <cell r="C708" t="str">
-            <v>Youngest Radiometric Age Ma</v>
+            <v>Younger Age URI</v>
           </cell>
         </row>
         <row r="709">
           <cell r="A709" t="str">
+            <v>class/attribute/youngestage</v>
+          </cell>
+          <cell r="C709" t="str">
+            <v>Youngest Age</v>
+          </cell>
+        </row>
+        <row r="710">
+          <cell r="A710" t="str">
+            <v>class/attribute/youngestradiometricage-ma</v>
+          </cell>
+          <cell r="C710" t="str">
+            <v>Youngest Radiometric Age Ma</v>
+          </cell>
+        </row>
+        <row r="711">
+          <cell r="A711" t="str">
             <v>class/attribute/zip</v>
           </cell>
-          <cell r="C709" t="str">
+          <cell r="C711" t="str">
             <v>Zip</v>
           </cell>
         </row>
@@ -7329,10 +7411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H363"/>
+  <dimension ref="A1:H406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G326" sqref="G326"/>
+    <sheetView tabSelected="1" topLeftCell="A378" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K396" sqref="K396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7682,7 +7764,7 @@
       </c>
       <c r="C14" s="15" t="str">
         <f>LOOKUP(D14,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
-        <v>Total Slip</v>
+        <v>Township</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>34</v>
@@ -7707,7 +7789,7 @@
       </c>
       <c r="C15" s="15" t="str">
         <f>LOOKUP(D15,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
-        <v>Radioactivity Measurement Device</v>
+        <v>Range</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>35</v>
@@ -16299,6 +16381,1081 @@
         <v>34</v>
       </c>
       <c r="G363" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="364" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A364" s="15" t="str">
+        <f>LOOKUP(B364,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B364" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C364" s="15" t="str">
+        <f>LOOKUP(D364,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>OBJECTID</v>
+      </c>
+      <c r="D364" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E364" s="6">
+        <v>1</v>
+      </c>
+      <c r="F364" s="5">
+        <v>1</v>
+      </c>
+      <c r="G364" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="365" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A365" s="15" t="str">
+        <f>LOOKUP(B365,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B365" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C365" s="15" t="str">
+        <f>LOOKUP(D365,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Thermal Spring URI</v>
+      </c>
+      <c r="D365" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="E365" s="6">
+        <v>1</v>
+      </c>
+      <c r="F365" s="5">
+        <v>2</v>
+      </c>
+      <c r="G365" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="366" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A366" s="15" t="str">
+        <f>LOOKUP(B366,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B366" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C366" s="15" t="str">
+        <f>LOOKUP(D366,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Spring Name</v>
+      </c>
+      <c r="D366" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="E366" s="6">
+        <v>1</v>
+      </c>
+      <c r="F366" s="5">
+        <v>3</v>
+      </c>
+      <c r="G366" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="367" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A367" s="15" t="str">
+        <f>LOOKUP(B367,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B367" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C367" s="15" t="str">
+        <f>LOOKUP(D367,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Label</v>
+      </c>
+      <c r="D367" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E367" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F367" s="5">
+        <v>4</v>
+      </c>
+      <c r="G367" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="368" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A368" s="15" t="str">
+        <f>LOOKUP(B368,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B368" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C368" s="15" t="str">
+        <f>LOOKUP(D368,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Other Name</v>
+      </c>
+      <c r="D368" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="E368" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F368" s="5">
+        <v>5</v>
+      </c>
+      <c r="G368" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A369" s="15" t="str">
+        <f>LOOKUP(B369,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B369" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C369" s="15" t="str">
+        <f>LOOKUP(D369,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Other Identifier</v>
+      </c>
+      <c r="D369" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="E369" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F369" s="5">
+        <v>6</v>
+      </c>
+      <c r="G369" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="370" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A370" s="15" t="str">
+        <f>LOOKUP(B370,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B370" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C370" s="15" t="str">
+        <f>LOOKUP(D370,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Description</v>
+      </c>
+      <c r="D370" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="E370" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F370" s="5">
+        <v>7</v>
+      </c>
+      <c r="G370" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A371" s="15" t="str">
+        <f>LOOKUP(B371,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B371" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C371" s="15" t="str">
+        <f>LOOKUP(D371,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Source</v>
+      </c>
+      <c r="D371" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E371" s="6">
+        <v>1</v>
+      </c>
+      <c r="F371" s="5">
+        <v>8</v>
+      </c>
+      <c r="G371" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="372" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A372" s="15" t="str">
+        <f>LOOKUP(B372,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B372" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C372" s="15" t="str">
+        <f>LOOKUP(D372,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Source URI</v>
+      </c>
+      <c r="D372" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="E372" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F372" s="5">
+        <v>9</v>
+      </c>
+      <c r="G372" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A373" s="15" t="str">
+        <f>LOOKUP(B373,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B373" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C373" s="15" t="str">
+        <f>LOOKUP(D373,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Feature Type</v>
+      </c>
+      <c r="D373" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="E373" s="6">
+        <v>1</v>
+      </c>
+      <c r="F373" s="5">
+        <v>10</v>
+      </c>
+      <c r="G373" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="374" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A374" s="15" t="str">
+        <f>LOOKUP(B374,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B374" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C374" s="15" t="str">
+        <f>LOOKUP(D374,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Land Lease Owner</v>
+      </c>
+      <c r="D374" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="E374" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F374" s="5">
+        <v>11</v>
+      </c>
+      <c r="G374" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="375" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A375" s="15" t="str">
+        <f>LOOKUP(B375,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B375" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C375" s="15" t="str">
+        <f>LOOKUP(D375,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Other Location Name</v>
+      </c>
+      <c r="D375" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="E375" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F375" s="5">
+        <v>12</v>
+      </c>
+      <c r="G375" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="376" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A376" s="15" t="str">
+        <f>LOOKUP(B376,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B376" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C376" s="15" t="str">
+        <f>LOOKUP(D376,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>County</v>
+      </c>
+      <c r="D376" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E376" s="6">
+        <v>1</v>
+      </c>
+      <c r="F376" s="5">
+        <v>13</v>
+      </c>
+      <c r="G376" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="377" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A377" s="15" t="str">
+        <f>LOOKUP(B377,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B377" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C377" s="15" t="str">
+        <f>LOOKUP(D377,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>State</v>
+      </c>
+      <c r="D377" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E377" s="6">
+        <v>1</v>
+      </c>
+      <c r="F377" s="5">
+        <v>14</v>
+      </c>
+      <c r="G377" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A378" s="15" t="str">
+        <f>LOOKUP(B378,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B378" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C378" s="15" t="str">
+        <f>LOOKUP(D378,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>PLSS Meridians</v>
+      </c>
+      <c r="D378" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E378" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F378" s="5">
+        <v>15</v>
+      </c>
+      <c r="G378" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="379" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A379" s="15" t="str">
+        <f>LOOKUP(B379,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B379" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C379" s="15" t="str">
+        <f>LOOKUP(D379,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Township</v>
+      </c>
+      <c r="D379" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E379" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F379" s="5">
+        <v>16</v>
+      </c>
+      <c r="G379" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="380" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A380" s="15" t="str">
+        <f>LOOKUP(B380,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B380" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C380" s="15" t="str">
+        <f>LOOKUP(D380,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Range</v>
+      </c>
+      <c r="D380" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E380" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F380" s="5">
+        <v>17</v>
+      </c>
+      <c r="G380" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="381" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A381" s="15" t="str">
+        <f>LOOKUP(B381,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B381" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C381" s="15" t="str">
+        <f>LOOKUP(D381,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v xml:space="preserve">Section </v>
+      </c>
+      <c r="D381" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E381" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F381" s="5">
+        <v>18</v>
+      </c>
+      <c r="G381" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="382" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A382" s="15" t="str">
+        <f>LOOKUP(B382,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B382" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C382" s="15" t="str">
+        <f>LOOKUP(D382,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Section Part</v>
+      </c>
+      <c r="D382" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E382" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F382" s="5">
+        <v>19</v>
+      </c>
+      <c r="G382" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A383" s="15" t="str">
+        <f>LOOKUP(B383,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B383" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C383" s="15" t="str">
+        <f>LOOKUP(D383,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Parcel</v>
+      </c>
+      <c r="D383" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E383" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F383" s="5">
+        <v>20</v>
+      </c>
+      <c r="G383" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A384" s="15" t="str">
+        <f>LOOKUP(B384,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B384" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C384" s="15" t="str">
+        <f>LOOKUP(D384,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>UTM E</v>
+      </c>
+      <c r="D384" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E384" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F384" s="5">
+        <v>21</v>
+      </c>
+      <c r="G384" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="385" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A385" s="15" t="str">
+        <f>LOOKUP(B385,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B385" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C385" s="15" t="str">
+        <f>LOOKUP(D385,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>UTM N</v>
+      </c>
+      <c r="D385" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E385" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F385" s="5">
+        <v>22</v>
+      </c>
+      <c r="G385" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="386" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A386" s="15" t="str">
+        <f>LOOKUP(B386,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B386" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C386" s="15" t="str">
+        <f>LOOKUP(D386,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>UTM Datum Zone</v>
+      </c>
+      <c r="D386" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E386" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F386" s="5">
+        <v>23</v>
+      </c>
+      <c r="G386" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="387" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A387" s="15" t="str">
+        <f>LOOKUP(B387,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B387" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C387" s="15" t="str">
+        <f>LOOKUP(D387,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Latitude Degrees</v>
+      </c>
+      <c r="D387" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E387" s="6">
+        <v>1</v>
+      </c>
+      <c r="F387" s="5">
+        <v>24</v>
+      </c>
+      <c r="G387" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="388" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A388" s="15" t="str">
+        <f>LOOKUP(B388,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B388" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C388" s="15" t="str">
+        <f>LOOKUP(D388,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Longitude Degree</v>
+      </c>
+      <c r="D388" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E388" s="6">
+        <v>1</v>
+      </c>
+      <c r="F388" s="5">
+        <v>25</v>
+      </c>
+      <c r="G388" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="389" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A389" s="15" t="str">
+        <f>LOOKUP(B389,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B389" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C389" s="15" t="str">
+        <f>LOOKUP(D389,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>SRS</v>
+      </c>
+      <c r="D389" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E389" s="6">
+        <v>1</v>
+      </c>
+      <c r="F389" s="5">
+        <v>26</v>
+      </c>
+      <c r="G389" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="390" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A390" s="15" t="str">
+        <f>LOOKUP(B390,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B390" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C390" s="15" t="str">
+        <f>LOOKUP(D390,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Location Uncertainty Statement</v>
+      </c>
+      <c r="D390" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E390" s="6">
+        <v>1</v>
+      </c>
+      <c r="F390" s="5">
+        <v>27</v>
+      </c>
+      <c r="G390" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="391" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A391" s="15" t="str">
+        <f>LOOKUP(B391,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B391" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C391" s="15" t="str">
+        <f>LOOKUP(D391,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Temperature</v>
+      </c>
+      <c r="D391" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="E391" s="6">
+        <v>1</v>
+      </c>
+      <c r="F391" s="5">
+        <v>28</v>
+      </c>
+      <c r="G391" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="392" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A392" s="15" t="str">
+        <f>LOOKUP(B392,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B392" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C392" s="15" t="str">
+        <f>LOOKUP(D392,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Temperature Units</v>
+      </c>
+      <c r="D392" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="E392" s="6">
+        <v>1</v>
+      </c>
+      <c r="F392" s="5">
+        <v>29</v>
+      </c>
+      <c r="G392" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="393" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A393" s="15" t="str">
+        <f>LOOKUP(B393,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B393" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C393" s="15" t="str">
+        <f>LOOKUP(D393,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Temp Measurement Procedure</v>
+      </c>
+      <c r="D393" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="E393" s="6">
+        <v>1</v>
+      </c>
+      <c r="F393" s="5">
+        <v>30</v>
+      </c>
+      <c r="G393" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="394" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A394" s="15" t="str">
+        <f>LOOKUP(B394,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B394" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C394" s="15" t="str">
+        <f>LOOKUP(D394,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Temp Measurement Date Time</v>
+      </c>
+      <c r="D394" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="E394" s="6">
+        <v>1</v>
+      </c>
+      <c r="F394" s="5">
+        <v>31</v>
+      </c>
+      <c r="G394" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A395" s="15" t="str">
+        <f>LOOKUP(B395,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B395" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C395" s="15" t="str">
+        <f>LOOKUP(D395,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Flow</v>
+      </c>
+      <c r="D395" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="E395" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F395" s="5">
+        <v>32</v>
+      </c>
+      <c r="G395" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="396" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A396" s="15" t="str">
+        <f>LOOKUP(B396,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B396" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C396" s="15" t="str">
+        <f>LOOKUP(D396,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Flow Units</v>
+      </c>
+      <c r="D396" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="E396" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F396" s="5">
+        <v>33</v>
+      </c>
+      <c r="G396" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="397" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A397" s="15" t="str">
+        <f>LOOKUP(B397,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B397" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C397" s="15" t="str">
+        <f>LOOKUP(D397,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Flow Measurement Procedure</v>
+      </c>
+      <c r="D397" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="E397" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F397" s="5">
+        <v>34</v>
+      </c>
+      <c r="G397" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="398" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A398" s="15" t="str">
+        <f>LOOKUP(B398,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B398" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C398" s="15" t="str">
+        <f>LOOKUP(D398,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Flow Measurement Date Time</v>
+      </c>
+      <c r="D398" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="E398" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F398" s="5">
+        <v>35</v>
+      </c>
+      <c r="G398" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A399" s="15" t="str">
+        <f>LOOKUP(B399,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B399" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C399" s="15" t="str">
+        <f>LOOKUP(D399,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Measurement Source</v>
+      </c>
+      <c r="D399" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="E399" s="6">
+        <v>1</v>
+      </c>
+      <c r="F399" s="5">
+        <v>36</v>
+      </c>
+      <c r="G399" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="400" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A400" s="15" t="str">
+        <f>LOOKUP(B400,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B400" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C400" s="15" t="str">
+        <f>LOOKUP(D400,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Flow Continuity</v>
+      </c>
+      <c r="D400" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="E400" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F400" s="5">
+        <v>37</v>
+      </c>
+      <c r="G400" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="401" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A401" s="15" t="str">
+        <f>LOOKUP(B401,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B401" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C401" s="15" t="str">
+        <f>LOOKUP(D401,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Classification</v>
+      </c>
+      <c r="D401" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="E401" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F401" s="5">
+        <v>38</v>
+      </c>
+      <c r="G401" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="402" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A402" s="15" t="str">
+        <f>LOOKUP(B402,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B402" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C402" s="15" t="str">
+        <f>LOOKUP(D402,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Related Water Chemistry</v>
+      </c>
+      <c r="D402" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="E402" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F402" s="5">
+        <v>39</v>
+      </c>
+      <c r="G402" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="403" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A403" s="15" t="str">
+        <f>LOOKUP(B403,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B403" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C403" s="15" t="str">
+        <f>LOOKUP(D403,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Related Resources</v>
+      </c>
+      <c r="D403" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="E403" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F403" s="5">
+        <v>40</v>
+      </c>
+      <c r="G403" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="404" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A404" s="15" t="str">
+        <f>LOOKUP(B404,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B404" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C404" s="15" t="str">
+        <f>LOOKUP(D404,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Remarks</v>
+      </c>
+      <c r="D404" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="E404" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F404" s="5">
+        <v>41</v>
+      </c>
+      <c r="G404" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="405" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A405" s="15" t="str">
+        <f>LOOKUP(B405,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B405" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C405" s="15" t="str">
+        <f>LOOKUP(D405,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Notes</v>
+      </c>
+      <c r="D405" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E405" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F405" s="5">
+        <v>42</v>
+      </c>
+      <c r="G405" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="406" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A406" s="15" t="str">
+        <f>LOOKUP(B406,[1]DataObject!$A:$A,[1]DataObject!$B:$B)</f>
+        <v>Thermal Spring Occurrence</v>
+      </c>
+      <c r="B406" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="C406" s="15" t="str">
+        <f>LOOKUP(D406,[2]Attribute!$A:$A,[2]Attribute!$C:$C)</f>
+        <v>Shape</v>
+      </c>
+      <c r="D406" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="E406" s="6">
+        <v>1</v>
+      </c>
+      <c r="F406" s="5">
+        <v>43</v>
+      </c>
+      <c r="G406" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>